<commit_message>
why rejected HVAC waste always zero
</commit_message>
<xml_diff>
--- a/_2_cases_input_outputs/_08_CAPITOUL/DOE_Ref_MediumOffice_4B/vcwg_ep_saving/ver1.1/CAPITOUL_Bypass_2004_can_Averaged_temp_k_specHum_ratio_press_pa.xlsx
+++ b/_2_cases_input_outputs/_08_CAPITOUL/DOE_Ref_MediumOffice_4B/vcwg_ep_saving/ver1.1/CAPITOUL_Bypass_2004_can_Averaged_temp_k_specHum_ratio_press_pa.xlsx
@@ -422,13 +422,13 @@
         <v>38139.00347222222</v>
       </c>
       <c r="B3">
-        <v>290.1692281689665</v>
+        <v>289.939825046251</v>
       </c>
       <c r="C3">
         <v>0.0100285939811304</v>
       </c>
       <c r="D3">
-        <v>100320.9877109042</v>
+        <v>100321.0821306008</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -436,13 +436,13 @@
         <v>38139.00694444445</v>
       </c>
       <c r="B4">
-        <v>288.9195451075033</v>
+        <v>288.7972612261858</v>
       </c>
       <c r="C4">
-        <v>0.0100010861301899</v>
+        <v>0.009999735626723055</v>
       </c>
       <c r="D4">
-        <v>100321.888760868</v>
+        <v>100321.9514278131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -450,13 +450,13 @@
         <v>38139.01041666666</v>
       </c>
       <c r="B5">
-        <v>289.0510867248721</v>
+        <v>288.911050312919</v>
       </c>
       <c r="C5">
-        <v>0.01001613333341143</v>
+        <v>0.01001497101912757</v>
       </c>
       <c r="D5">
-        <v>100321.8387834093</v>
+        <v>100321.9145167599</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -464,13 +464,13 @@
         <v>38139.01388888889</v>
       </c>
       <c r="B6">
-        <v>289.3623103195695</v>
+        <v>289.2057976501019</v>
       </c>
       <c r="C6">
-        <v>0.01004720756219118</v>
+        <v>0.01004644782318701</v>
       </c>
       <c r="D6">
-        <v>100321.6676769431</v>
+        <v>100321.7581643073</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>38139.01736111111</v>
       </c>
       <c r="B7">
-        <v>289.3806175041194</v>
+        <v>289.1889808952836</v>
       </c>
       <c r="C7">
-        <v>0.01007568168461182</v>
+        <v>0.01007538861214716</v>
       </c>
       <c r="D7">
-        <v>100321.5870577408</v>
+        <v>100321.6968065166</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>38139.02083333334</v>
       </c>
       <c r="B8">
-        <v>289.5165474556151</v>
+        <v>289.3302917481501</v>
       </c>
       <c r="C8">
-        <v>0.01010249313942127</v>
+        <v>0.01010266587750968</v>
       </c>
       <c r="D8">
-        <v>100321.4649929776</v>
+        <v>100321.5765220945</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>38139.02430555555</v>
       </c>
       <c r="B9">
-        <v>289.4357340345404</v>
+        <v>289.6102451410316</v>
       </c>
       <c r="C9">
-        <v>0.01012514546404897</v>
+        <v>0.01015535635866254</v>
       </c>
       <c r="D9">
-        <v>100321.4232400307</v>
+        <v>100321.4449589966</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -520,13 +520,13 @@
         <v>38139.02777777778</v>
       </c>
       <c r="B10">
-        <v>289.5109052986889</v>
+        <v>289.8181879933676</v>
       </c>
       <c r="C10">
-        <v>0.01014891667821144</v>
+        <v>0.010217359140748</v>
       </c>
       <c r="D10">
-        <v>100321.3219713062</v>
+        <v>100321.3677160654</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -534,13 +534,13 @@
         <v>38139.03125</v>
       </c>
       <c r="B11">
-        <v>289.4310093916164</v>
+        <v>289.654032314757</v>
       </c>
       <c r="C11">
-        <v>0.01017266855617449</v>
+        <v>0.01027349500581297</v>
       </c>
       <c r="D11">
-        <v>100321.2660382831</v>
+        <v>100321.3542792998</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -548,13 +548,13 @@
         <v>38139.03472222222</v>
       </c>
       <c r="B12">
-        <v>289.5267812233168</v>
+        <v>289.786301055347</v>
       </c>
       <c r="C12">
-        <v>0.01020098113946412</v>
+        <v>0.01032357930489896</v>
       </c>
       <c r="D12">
-        <v>100321.1324437697</v>
+        <v>100321.2571748879</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -562,13 +562,13 @@
         <v>38139.03819444445</v>
       </c>
       <c r="B13">
-        <v>289.4738464509534</v>
+        <v>289.5745579383371</v>
       </c>
       <c r="C13">
-        <v>0.01023209088971142</v>
+        <v>0.01036654764857654</v>
       </c>
       <c r="D13">
-        <v>100321.033312179</v>
+        <v>100321.2436321805</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -576,13 +576,13 @@
         <v>38139.04166666666</v>
       </c>
       <c r="B14">
-        <v>289.5995461596182</v>
+        <v>289.703807703247</v>
       </c>
       <c r="C14">
-        <v>0.01026947064638757</v>
+        <v>0.01040674566029152</v>
       </c>
       <c r="D14">
-        <v>100320.8498882245</v>
+        <v>100321.1597510381</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -590,13 +590,13 @@
         <v>38139.04513888889</v>
       </c>
       <c r="B15">
-        <v>289.52321035852</v>
+        <v>289.4725414952485</v>
       </c>
       <c r="C15">
-        <v>0.01029035385813967</v>
+        <v>0.01044273597068787</v>
       </c>
       <c r="D15">
-        <v>100320.9199905575</v>
+        <v>100321.2014634013</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -604,13 +604,13 @@
         <v>38139.04861111111</v>
       </c>
       <c r="B16">
-        <v>289.5636591137605</v>
+        <v>289.6426262154588</v>
       </c>
       <c r="C16">
-        <v>0.01029288125298886</v>
+        <v>0.01047826651691994</v>
       </c>
       <c r="D16">
-        <v>100321.0163653639</v>
+        <v>100321.172242841</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -618,13 +618,13 @@
         <v>38139.05208333334</v>
       </c>
       <c r="B17">
-        <v>289.7486789131571</v>
+        <v>289.3794389223004</v>
       </c>
       <c r="C17">
-        <v>0.01032223405574956</v>
+        <v>0.01050746120980681</v>
       </c>
       <c r="D17">
-        <v>100321.0548418228</v>
+        <v>100321.2678264897</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -632,13 +632,13 @@
         <v>38139.05555555555</v>
       </c>
       <c r="B18">
-        <v>289.9937804260866</v>
+        <v>289.571267360429</v>
       </c>
       <c r="C18">
-        <v>0.01036522119414165</v>
+        <v>0.01053251941820298</v>
       </c>
       <c r="D18">
-        <v>100321.1000580329</v>
+        <v>100321.2994067744</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -646,13 +646,13 @@
         <v>38139.05902777778</v>
       </c>
       <c r="B19">
-        <v>289.8830568951317</v>
+        <v>289.26164972913</v>
       </c>
       <c r="C19">
-        <v>0.010403649554523</v>
+        <v>0.01054675123519587</v>
       </c>
       <c r="D19">
-        <v>100321.2089781025</v>
+        <v>100321.4749678989</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -660,13 +660,13 @@
         <v>38139.0625</v>
       </c>
       <c r="B20">
-        <v>290.0280936963878</v>
+        <v>289.4676186882333</v>
       </c>
       <c r="C20">
-        <v>0.01043682760121891</v>
+        <v>0.01055459555927396</v>
       </c>
       <c r="D20">
-        <v>100321.2597380551</v>
+        <v>100321.5492488659</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -674,13 +674,13 @@
         <v>38139.06597222222</v>
       </c>
       <c r="B21">
-        <v>289.8468013279112</v>
+        <v>289.1060341825254</v>
       </c>
       <c r="C21">
-        <v>0.01045921724301822</v>
+        <v>0.01054879383309737</v>
       </c>
       <c r="D21">
-        <v>100321.3868082464</v>
+        <v>100321.7557694002</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -688,13 +688,13 @@
         <v>38139.06944444445</v>
       </c>
       <c r="B22">
-        <v>289.9564324860841</v>
+        <v>289.3366838498188</v>
       </c>
       <c r="C22">
-        <v>0.01047372023080858</v>
+        <v>0.01053569613807139</v>
       </c>
       <c r="D22">
-        <v>100321.452281587</v>
+        <v>100321.8243848731</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -702,13 +702,13 @@
         <v>38139.07291666666</v>
       </c>
       <c r="B23">
-        <v>289.7384644586088</v>
+        <v>288.9397134581743</v>
       </c>
       <c r="C23">
-        <v>0.01047757503976282</v>
+        <v>0.01051246044669953</v>
       </c>
       <c r="D23">
-        <v>100321.589809283</v>
+        <v>100322.0258907562</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -716,13 +716,13 @@
         <v>38139.07638888889</v>
       </c>
       <c r="B24">
-        <v>289.8530282031732</v>
+        <v>289.2200079937942</v>
       </c>
       <c r="C24">
-        <v>0.01047607745519579</v>
+        <v>0.01048764461636115</v>
       </c>
       <c r="D24">
-        <v>100321.6531592506</v>
+        <v>100322.0645745295</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -730,13 +730,13 @@
         <v>38139.07986111111</v>
       </c>
       <c r="B25">
-        <v>289.6142085150645</v>
+        <v>288.7950990082052</v>
       </c>
       <c r="C25">
-        <v>0.01046563319572275</v>
+        <v>0.01045654634004272</v>
       </c>
       <c r="D25">
-        <v>100321.7907434977</v>
+        <v>100322.2545529135</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -744,13 +744,13 @@
         <v>38139.08333333334</v>
       </c>
       <c r="B26">
-        <v>289.7458384550681</v>
+        <v>289.1294842873755</v>
       </c>
       <c r="C26">
-        <v>0.01045237950164614</v>
+        <v>0.01042628388762553</v>
       </c>
       <c r="D26">
-        <v>100321.8439334514</v>
+        <v>100322.2657036971</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -758,13 +758,13 @@
         <v>38139.08680555555</v>
       </c>
       <c r="B27">
-        <v>289.5000289978016</v>
+        <v>288.6759612524412</v>
       </c>
       <c r="C27">
-        <v>0.010434259887096</v>
+        <v>0.01039226813949958</v>
       </c>
       <c r="D27">
-        <v>100321.9372003011</v>
+        <v>100322.4156039193</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -772,13 +772,13 @@
         <v>38139.09027777778</v>
       </c>
       <c r="B28">
-        <v>289.6706913975716</v>
+        <v>289.0775654926273</v>
       </c>
       <c r="C28">
-        <v>0.01041850790804495</v>
+        <v>0.01036407449643263</v>
       </c>
       <c r="D28">
-        <v>100321.9205904698</v>
+        <v>100322.35458621</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -786,13 +786,13 @@
         <v>38139.09375</v>
       </c>
       <c r="B29">
-        <v>289.425957894748</v>
+        <v>288.5960797164429</v>
       </c>
       <c r="C29">
-        <v>0.01040206095777731</v>
+        <v>0.01033267451475205</v>
       </c>
       <c r="D29">
-        <v>100321.9816947067</v>
+        <v>100322.4836889711</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -800,13 +800,13 @@
         <v>38139.09722222222</v>
       </c>
       <c r="B30">
-        <v>289.6349319656852</v>
+        <v>289.0617128701992</v>
       </c>
       <c r="C30">
-        <v>0.01038989258940302</v>
+        <v>0.01031015926992742</v>
       </c>
       <c r="D30">
-        <v>100321.9368902618</v>
+        <v>100322.3910526204</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -814,13 +814,13 @@
         <v>38139.10069444445</v>
       </c>
       <c r="B31">
-        <v>289.3856763443296</v>
+        <v>288.5458709540567</v>
       </c>
       <c r="C31">
-        <v>0.01037362295511731</v>
+        <v>0.01028318556314564</v>
       </c>
       <c r="D31">
-        <v>100321.9870927607</v>
+        <v>100322.5167295693</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -828,13 +828,13 @@
         <v>38139.10416666666</v>
       </c>
       <c r="B32">
-        <v>289.6253539149396</v>
+        <v>289.0695488756713</v>
       </c>
       <c r="C32">
-        <v>0.01035939597596501</v>
+        <v>0.01026291772568866</v>
       </c>
       <c r="D32">
-        <v>100321.9287921243</v>
+        <v>100322.4027857056</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -842,13 +842,13 @@
         <v>38139.10763888889</v>
       </c>
       <c r="B33">
-        <v>289.3637432708423</v>
+        <v>288.5148373570458</v>
       </c>
       <c r="C33">
-        <v>0.01034312740380821</v>
+        <v>0.01023753956988816</v>
       </c>
       <c r="D33">
-        <v>100321.9772615448</v>
+        <v>100322.5307436255</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -856,13 +856,13 @@
         <v>38139.11111111111</v>
       </c>
       <c r="B34">
-        <v>289.6294494474517</v>
+        <v>289.0907244265688</v>
       </c>
       <c r="C34">
-        <v>0.01033152698520241</v>
+        <v>0.01022157157649864</v>
       </c>
       <c r="D34">
-        <v>100321.9103858817</v>
+        <v>100322.398893097</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -870,13 +870,13 @@
         <v>38139.11458333334</v>
       </c>
       <c r="B35">
-        <v>289.3535181913388</v>
+        <v>288.4967711129627</v>
       </c>
       <c r="C35">
-        <v>0.01031956811878287</v>
+        <v>0.01020031822684754</v>
       </c>
       <c r="D35">
-        <v>100321.9590705534</v>
+        <v>100322.5293319837</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -884,13 +884,13 @@
         <v>38139.11805555555</v>
       </c>
       <c r="B36">
-        <v>289.6439547434699</v>
+        <v>289.1207247501904</v>
       </c>
       <c r="C36">
-        <v>0.01031281811748367</v>
+        <v>0.01018906108619752</v>
       </c>
       <c r="D36">
-        <v>100321.884499186</v>
+        <v>100322.3803413419</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -898,13 +898,13 @@
         <v>38139.12152777778</v>
       </c>
       <c r="B37">
-        <v>289.3534885935489</v>
+        <v>288.4907062395338</v>
       </c>
       <c r="C37">
-        <v>0.01030590922903505</v>
+        <v>0.01017183159809584</v>
       </c>
       <c r="D37">
-        <v>100321.9336370814</v>
+        <v>100322.5126255751</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -912,13 +912,13 @@
         <v>38139.125</v>
       </c>
       <c r="B38">
-        <v>289.6676543545608</v>
+        <v>289.1580073239299</v>
       </c>
       <c r="C38">
-        <v>0.01030473648825952</v>
+        <v>0.01016650971542686</v>
       </c>
       <c r="D38">
-        <v>100321.8518088287</v>
+        <v>100322.348243445</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -926,13 +926,13 @@
         <v>38139.12847222222</v>
       </c>
       <c r="B39">
-        <v>289.359367352392</v>
+        <v>288.4916593040861</v>
       </c>
       <c r="C39">
-        <v>0.01030205435632683</v>
+        <v>0.01015373793460457</v>
       </c>
       <c r="D39">
-        <v>100321.8811905656</v>
+        <v>100322.4696629537</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -940,13 +940,13 @@
         <v>38139.13194444445</v>
       </c>
       <c r="B40">
-        <v>289.6911769337693</v>
+        <v>289.1885594054158</v>
       </c>
       <c r="C40">
-        <v>0.01030480319452958</v>
+        <v>0.01015344056120964</v>
       </c>
       <c r="D40">
-        <v>100321.7646428098</v>
+        <v>100322.2815044482</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -954,13 +954,13 @@
         <v>38139.13541666666</v>
       </c>
       <c r="B41">
-        <v>289.3651746763995</v>
+        <v>288.4870908312078</v>
       </c>
       <c r="C41">
-        <v>0.01030241281783067</v>
+        <v>0.01014308180842039</v>
       </c>
       <c r="D41">
-        <v>100321.7829008729</v>
+        <v>100322.4148003384</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -968,13 +968,13 @@
         <v>38139.13888888889</v>
       </c>
       <c r="B42">
-        <v>289.7176742330108</v>
+        <v>289.2111723549664</v>
       </c>
       <c r="C42">
-        <v>0.0103031079148863</v>
+        <v>0.01014358869952064</v>
       </c>
       <c r="D42">
-        <v>100321.6531875329</v>
+        <v>100322.2205696831</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -982,13 +982,13 @@
         <v>38139.14236111111</v>
       </c>
       <c r="B43">
-        <v>289.3746594613518</v>
+        <v>288.4811946118494</v>
       </c>
       <c r="C43">
-        <v>0.0103001335949373</v>
+        <v>0.01013360384442818</v>
       </c>
       <c r="D43">
-        <v>100321.6697584655</v>
+        <v>100322.3539556633</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -996,13 +996,13 @@
         <v>38139.14583333334</v>
       </c>
       <c r="B44">
-        <v>289.74645572347</v>
+        <v>289.2295531370147</v>
       </c>
       <c r="C44">
-        <v>0.01030328118276471</v>
+        <v>0.01013551747967288</v>
       </c>
       <c r="D44">
-        <v>100321.5332055662</v>
+        <v>100322.1521485548</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1010,13 +1010,13 @@
         <v>38139.14930555555</v>
       </c>
       <c r="B45">
-        <v>289.3853075393274</v>
+        <v>288.4760041405807</v>
       </c>
       <c r="C45">
-        <v>0.01029413979842631</v>
+        <v>0.01012591014849353</v>
       </c>
       <c r="D45">
-        <v>100321.5516304067</v>
+        <v>100322.2877614358</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1024,13 +1024,13 @@
         <v>38139.15277777778</v>
       </c>
       <c r="B46">
-        <v>289.7746060522374</v>
+        <v>289.2434033072602</v>
       </c>
       <c r="C46">
-        <v>0.01029285023375898</v>
+        <v>0.01013038359561325</v>
       </c>
       <c r="D46">
-        <v>100321.4102376543</v>
+        <v>100322.0800075043</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1038,13 +1038,13 @@
         <v>38139.15625</v>
       </c>
       <c r="B47">
-        <v>289.3959115226627</v>
+        <v>288.4718268461995</v>
       </c>
       <c r="C47">
-        <v>0.01028768461368169</v>
+        <v>0.01012222789035066</v>
       </c>
       <c r="D47">
-        <v>100321.4309295058</v>
+        <v>100322.2172914045</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1052,13 +1052,13 @@
         <v>38139.15972222222</v>
       </c>
       <c r="B48">
-        <v>289.8018882626745</v>
+        <v>289.2534717449309</v>
       </c>
       <c r="C48">
-        <v>0.01029181794901278</v>
+        <v>0.01012921966252004</v>
       </c>
       <c r="D48">
-        <v>100321.2850192982</v>
+        <v>100322.0053663537</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1066,13 +1066,13 @@
         <v>38139.16319444445</v>
       </c>
       <c r="B49">
-        <v>289.4071451671446</v>
+        <v>288.4694057322935</v>
       </c>
       <c r="C49">
-        <v>0.01028732745341193</v>
+        <v>0.01012122255517135</v>
       </c>
       <c r="D49">
-        <v>100321.3076689516</v>
+        <v>100322.1433919851</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1080,13 +1080,13 @@
         <v>38139.16666666666</v>
       </c>
       <c r="B50">
-        <v>289.8278975165326</v>
+        <v>289.2601864950396</v>
       </c>
       <c r="C50">
-        <v>0.01029008628420955</v>
+        <v>0.0101288694069711</v>
       </c>
       <c r="D50">
-        <v>100321.1579505475</v>
+        <v>100321.9283293464</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1094,13 +1094,13 @@
         <v>38139.17013888889</v>
       </c>
       <c r="B51">
-        <v>289.4089768302001</v>
+        <v>288.4632861907344</v>
       </c>
       <c r="C51">
-        <v>0.01028294416839954</v>
+        <v>0.0101192704978283</v>
       </c>
       <c r="D51">
-        <v>100321.2779354627</v>
+        <v>100322.1119331408</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1108,13 +1108,13 @@
         <v>38139.17361111111</v>
       </c>
       <c r="B52">
-        <v>289.825480863016</v>
+        <v>289.2528514667779</v>
       </c>
       <c r="C52">
-        <v>0.01028274983156819</v>
+        <v>0.01012473951550067</v>
       </c>
       <c r="D52">
-        <v>100321.2658145919</v>
+        <v>100321.9589478394</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1122,13 +1122,13 @@
         <v>38139.17708333334</v>
       </c>
       <c r="B53">
-        <v>289.360183326448</v>
+        <v>288.4350578499816</v>
       </c>
       <c r="C53">
-        <v>0.01027236132554256</v>
+        <v>0.01011198227073283</v>
       </c>
       <c r="D53">
-        <v>100321.4656430567</v>
+        <v>100322.1698371046</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1136,13 +1136,13 @@
         <v>38139.18055555555</v>
       </c>
       <c r="B54">
-        <v>289.764107078876</v>
+        <v>289.2222478970967</v>
       </c>
       <c r="C54">
-        <v>0.01026596144007445</v>
+        <v>0.0101135815523312</v>
       </c>
       <c r="D54">
-        <v>100321.4889720379</v>
+        <v>100322.0336277953</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1150,13 +1150,13 @@
         <v>38139.18402777778</v>
       </c>
       <c r="B55">
-        <v>289.257401241001</v>
+        <v>288.3826878547233</v>
       </c>
       <c r="C55">
-        <v>0.01024635151764501</v>
+        <v>0.01009360586542038</v>
       </c>
       <c r="D55">
-        <v>100321.6963104116</v>
+        <v>100322.2736524736</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1164,13 +1164,13 @@
         <v>38139.1875</v>
       </c>
       <c r="B56">
-        <v>289.6704583973185</v>
+        <v>289.1660072584451</v>
       </c>
       <c r="C56">
-        <v>0.010232369045906</v>
+        <v>0.0100874280586196</v>
       </c>
       <c r="D56">
-        <v>100321.6976106719</v>
+        <v>100322.1583481002</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1178,13 +1178,13 @@
         <v>38139.19097222222</v>
       </c>
       <c r="B57">
-        <v>289.1408661298536</v>
+        <v>288.3085958108321</v>
       </c>
       <c r="C57">
-        <v>0.0102071143965656</v>
+        <v>0.0100588498341603</v>
       </c>
       <c r="D57">
-        <v>100321.8861248916</v>
+        <v>100322.412285966</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1192,13 +1192,13 @@
         <v>38139.19444444445</v>
       </c>
       <c r="B58">
-        <v>289.5806106749236</v>
+        <v>289.0950693473868</v>
       </c>
       <c r="C58">
-        <v>0.01018962490667597</v>
+        <v>0.0100457760627608</v>
       </c>
       <c r="D58">
-        <v>100321.8600118569</v>
+        <v>100322.2965445945</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1206,13 +1206,13 @@
         <v>38139.19791666666</v>
       </c>
       <c r="B59">
-        <v>289.0297708231229</v>
+        <v>288.2257445397304</v>
       </c>
       <c r="C59">
-        <v>0.01016814819595158</v>
+        <v>0.01001526003071058</v>
       </c>
       <c r="D59">
-        <v>100322.0374634296</v>
+        <v>100322.5507264939</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1220,13 +1220,13 @@
         <v>38139.20138888889</v>
       </c>
       <c r="B60">
-        <v>289.4946400093253</v>
+        <v>289.0204145018988</v>
       </c>
       <c r="C60">
-        <v>0.01016084532242664</v>
+        <v>0.01000607289901818</v>
       </c>
       <c r="D60">
-        <v>100321.993532806</v>
+        <v>100322.4265544597</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1234,13 +1234,13 @@
         <v>38139.20486111111</v>
       </c>
       <c r="B61">
-        <v>288.9186065655407</v>
+        <v>288.1424346215716</v>
       </c>
       <c r="C61">
-        <v>0.01014412935580303</v>
+        <v>0.009976277285991601</v>
       </c>
       <c r="D61">
-        <v>100322.1680075913</v>
+        <v>100322.6779796733</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1248,13 +1248,13 @@
         <v>38139.20833333334</v>
       </c>
       <c r="B62">
-        <v>289.4084710106112</v>
+        <v>288.9455662684447</v>
       </c>
       <c r="C62">
-        <v>0.01013333714678178</v>
+        <v>0.009966404440645608</v>
       </c>
       <c r="D62">
-        <v>100322.1111698894</v>
+        <v>100322.5450720258</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1262,13 +1262,13 @@
         <v>38139.21180555555</v>
       </c>
       <c r="B63">
-        <v>288.8106294670103</v>
+        <v>288.0645223864764</v>
       </c>
       <c r="C63">
-        <v>0.01011229533170589</v>
+        <v>0.009934823748231654</v>
       </c>
       <c r="D63">
-        <v>100322.3106305321</v>
+        <v>100322.8149619238</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1276,13 +1276,13 @@
         <v>38139.21527777778</v>
       </c>
       <c r="B64">
-        <v>289.3329671446656</v>
+        <v>288.8848161296304</v>
       </c>
       <c r="C64">
-        <v>0.01009783680659932</v>
+        <v>0.009924578382797214</v>
       </c>
       <c r="D64">
-        <v>100322.2699495504</v>
+        <v>100322.6943721784</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1290,13 +1290,13 @@
         <v>38139.21875</v>
       </c>
       <c r="B65">
-        <v>288.7178378066749</v>
+        <v>288.0077367193117</v>
       </c>
       <c r="C65">
-        <v>0.01008148808895168</v>
+        <v>0.009897041708907778</v>
       </c>
       <c r="D65">
-        <v>100322.4691626265</v>
+        <v>100322.9565610555</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1304,13 +1304,13 @@
         <v>38139.22222222222</v>
       </c>
       <c r="B66">
-        <v>289.2682522139499</v>
+        <v>288.8357115689388</v>
       </c>
       <c r="C66">
-        <v>0.01007778244394575</v>
+        <v>0.00989735184617559</v>
       </c>
       <c r="D66">
-        <v>100322.4093506463</v>
+        <v>100322.8193206968</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1318,13 +1318,13 @@
         <v>38139.22569444445</v>
       </c>
       <c r="B67">
-        <v>288.6365830154781</v>
+        <v>287.9638134083257</v>
       </c>
       <c r="C67">
-        <v>0.01006674904107236</v>
+        <v>0.009875274488269444</v>
       </c>
       <c r="D67">
-        <v>100322.6013530474</v>
+        <v>100323.0713153822</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1332,13 +1332,13 @@
         <v>38139.22916666666</v>
       </c>
       <c r="B68">
-        <v>289.2579358364011</v>
+        <v>288.8321383426959</v>
       </c>
       <c r="C68">
-        <v>0.01006651044489261</v>
+        <v>0.009871626773262723</v>
       </c>
       <c r="D68">
-        <v>100322.5341740387</v>
+        <v>100322.9509004626</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1346,13 +1346,13 @@
         <v>38139.23263888889</v>
       </c>
       <c r="B69">
-        <v>288.5041664364508</v>
+        <v>287.8867294290279</v>
       </c>
       <c r="C69">
-        <v>0.01004710885054079</v>
+        <v>0.009818435726689629</v>
       </c>
       <c r="D69">
-        <v>100322.7270817545</v>
+        <v>100323.2071802225</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1360,13 +1360,13 @@
         <v>38139.23611111111</v>
       </c>
       <c r="B70">
-        <v>289.2012215051713</v>
+        <v>288.7855599181399</v>
       </c>
       <c r="C70">
-        <v>0.01005450756971444</v>
+        <v>0.009838511161279435</v>
       </c>
       <c r="D70">
-        <v>100322.620042564</v>
+        <v>100323.023994006</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1374,13 +1374,13 @@
         <v>38139.23958333334</v>
       </c>
       <c r="B71">
-        <v>288.4436874716115</v>
+        <v>287.8825930905083</v>
       </c>
       <c r="C71">
-        <v>0.01005611922298724</v>
+        <v>0.009818360179713888</v>
       </c>
       <c r="D71">
-        <v>100322.8002759282</v>
+        <v>100323.2409141851</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1388,13 +1388,13 @@
         <v>38139.24305555555</v>
       </c>
       <c r="B72">
-        <v>288.6957067496123</v>
+        <v>288.787557223641</v>
       </c>
       <c r="C72">
-        <v>0.009991330492765873</v>
+        <v>0.009857813080086732</v>
       </c>
       <c r="D72">
-        <v>100322.7983222429</v>
+        <v>100323.0261747822</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1402,13 +1402,13 @@
         <v>38139.24652777778</v>
       </c>
       <c r="B73">
-        <v>288.0984378720288</v>
+        <v>287.9318369038349</v>
       </c>
       <c r="C73">
-        <v>0.009933905405527571</v>
+        <v>0.009850855790056644</v>
       </c>
       <c r="D73">
-        <v>100322.9607825498</v>
+        <v>100323.2192918036</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1416,13 +1416,13 @@
         <v>38139.25</v>
       </c>
       <c r="B74">
-        <v>288.6065244163882</v>
+        <v>288.8344515683896</v>
       </c>
       <c r="C74">
-        <v>0.009949111690453812</v>
+        <v>0.009913145436032124</v>
       </c>
       <c r="D74">
-        <v>100322.8759809363</v>
+        <v>100322.9924732318</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1430,13 +1430,13 @@
         <v>38139.25347222222</v>
       </c>
       <c r="B75">
-        <v>287.8716969528833</v>
+        <v>288.0114400658459</v>
       </c>
       <c r="C75">
-        <v>0.009920369123000702</v>
+        <v>0.009926202421649174</v>
       </c>
       <c r="D75">
-        <v>100323.1358683744</v>
+        <v>100323.1902859748</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1444,13 +1444,13 @@
         <v>38139.25694444445</v>
       </c>
       <c r="B76">
-        <v>288.1716084923797</v>
+        <v>288.4460108163195</v>
       </c>
       <c r="C76">
-        <v>0.009898429267658914</v>
+        <v>0.009942317268581103</v>
       </c>
       <c r="D76">
-        <v>100323.0799684487</v>
+        <v>100323.0898680597</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1458,13 +1458,13 @@
         <v>38139.26041666666</v>
       </c>
       <c r="B77">
-        <v>287.9232993077205</v>
+        <v>287.6110607619954</v>
       </c>
       <c r="C77">
-        <v>0.009875874945286073</v>
+        <v>0.009874491163002565</v>
       </c>
       <c r="D77">
-        <v>100323.2161839911</v>
+        <v>100323.3769224244</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1472,13 +1472,13 @@
         <v>38139.26388888889</v>
       </c>
       <c r="B78">
-        <v>288.2533870731896</v>
+        <v>288.1219931845961</v>
       </c>
       <c r="C78">
-        <v>0.009902386894346216</v>
+        <v>0.009918215941019659</v>
       </c>
       <c r="D78">
-        <v>100323.1314558957</v>
+        <v>100323.225141612</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1486,13 +1486,13 @@
         <v>38139.26736111111</v>
       </c>
       <c r="B79">
-        <v>287.9744709134856</v>
+        <v>287.7706384472331</v>
       </c>
       <c r="C79">
-        <v>0.009905202519804346</v>
+        <v>0.009926309253131021</v>
       </c>
       <c r="D79">
-        <v>100323.2654618273</v>
+        <v>100323.3879861451</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1500,13 +1500,13 @@
         <v>38139.27083333334</v>
       </c>
       <c r="B80">
-        <v>288.2790377605222</v>
+        <v>288.2575029755909</v>
       </c>
       <c r="C80">
-        <v>0.009892870796106703</v>
+        <v>0.009934226294323036</v>
       </c>
       <c r="D80">
-        <v>100323.1949047993</v>
+        <v>100323.2452211843</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1514,13 +1514,13 @@
         <v>38139.27430555555</v>
       </c>
       <c r="B81">
-        <v>287.9871497555027</v>
+        <v>287.8093224233294</v>
       </c>
       <c r="C81">
-        <v>0.009912699625560269</v>
+        <v>0.009962785649656435</v>
       </c>
       <c r="D81">
-        <v>100323.3319678316</v>
+        <v>100323.4262462109</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1528,13 +1528,13 @@
         <v>38139.27777777778</v>
       </c>
       <c r="B82">
-        <v>288.3044448602993</v>
+        <v>288.3858543156841</v>
       </c>
       <c r="C82">
-        <v>0.009915209129154438</v>
+        <v>0.009996194789421316</v>
       </c>
       <c r="D82">
-        <v>100323.2549635895</v>
+        <v>100323.2491862638</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1542,13 +1542,13 @@
         <v>38139.28125</v>
       </c>
       <c r="B83">
-        <v>288.0296438602564</v>
+        <v>287.9500655925451</v>
       </c>
       <c r="C83">
-        <v>0.009899133464640376</v>
+        <v>0.01000388137988612</v>
       </c>
       <c r="D83">
-        <v>100323.3789891623</v>
+        <v>100323.4146470712</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1556,13 +1556,13 @@
         <v>38139.28472222222</v>
       </c>
       <c r="B84">
-        <v>288.3623274862701</v>
+        <v>288.5888125324522</v>
       </c>
       <c r="C84">
-        <v>0.009874941756824528</v>
+        <v>0.0100292027917062</v>
       </c>
       <c r="D84">
-        <v>100323.2942248183</v>
+        <v>100323.213511092</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1570,13 +1570,13 @@
         <v>38139.28819444445</v>
       </c>
       <c r="B85">
-        <v>288.0927670405792</v>
+        <v>288.1327237384681</v>
       </c>
       <c r="C85">
-        <v>0.00989321268114295</v>
+        <v>0.01007508192416275</v>
       </c>
       <c r="D85">
-        <v>100323.4108168904</v>
+        <v>100323.365847212</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1584,13 +1584,13 @@
         <v>38139.29166666666</v>
       </c>
       <c r="B86">
-        <v>288.431741052448</v>
+        <v>288.7875682422984</v>
       </c>
       <c r="C86">
-        <v>0.009895781714102454</v>
+        <v>0.01012999918456626</v>
       </c>
       <c r="D86">
-        <v>100323.3237343181</v>
+        <v>100323.165913019</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1598,13 +1598,13 @@
         <v>38139.29513888889</v>
       </c>
       <c r="B87">
-        <v>288.1681957497512</v>
+        <v>288.3151231906801</v>
       </c>
       <c r="C87">
-        <v>0.009882541375512244</v>
+        <v>0.01015743979366449</v>
       </c>
       <c r="D87">
-        <v>100323.419234095</v>
+        <v>100323.2978546474</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1612,13 +1612,13 @@
         <v>38139.29861111111</v>
       </c>
       <c r="B88">
-        <v>288.5761411886833</v>
+        <v>288.9513969917906</v>
       </c>
       <c r="C88">
-        <v>0.009914720971936236</v>
+        <v>0.01018603209860246</v>
       </c>
       <c r="D88">
-        <v>100323.2768133119</v>
+        <v>100323.09552107</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1626,13 +1626,13 @@
         <v>38139.30208333334</v>
       </c>
       <c r="B89">
-        <v>288.3634625578439</v>
+        <v>288.2460959827104</v>
       </c>
       <c r="C89">
-        <v>0.009924989522875063</v>
+        <v>0.01004395837565753</v>
       </c>
       <c r="D89">
-        <v>100323.3254401246</v>
+        <v>100323.3736192353</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1640,13 +1640,13 @@
         <v>38139.30555555555</v>
       </c>
       <c r="B90">
-        <v>288.8350201375017</v>
+        <v>288.7244458691822</v>
       </c>
       <c r="C90">
-        <v>0.009932641945796603</v>
+        <v>0.009982128917503334</v>
       </c>
       <c r="D90">
-        <v>100323.1466317091</v>
+        <v>100323.2099976942</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1654,13 +1654,13 @@
         <v>38139.30902777778</v>
       </c>
       <c r="B91">
-        <v>288.6187663728743</v>
+        <v>288.4050222641557</v>
       </c>
       <c r="C91">
-        <v>0.009959354459790111</v>
+        <v>0.009970181848817141</v>
       </c>
       <c r="D91">
-        <v>100323.1757415299</v>
+        <v>100323.2994189474</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1668,13 +1668,13 @@
         <v>38139.3125</v>
       </c>
       <c r="B92">
-        <v>289.1262032155314</v>
+        <v>289.0581843207556</v>
       </c>
       <c r="C92">
-        <v>0.009990068322484565</v>
+        <v>0.0099999663934538</v>
       </c>
       <c r="D92">
-        <v>100322.977800409</v>
+        <v>100323.0562199043</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1682,13 +1682,13 @@
         <v>38139.31597222222</v>
       </c>
       <c r="B93">
-        <v>288.914329297604</v>
+        <v>288.6394982410757</v>
       </c>
       <c r="C93">
-        <v>0.009988164951576972</v>
+        <v>0.009973334045439684</v>
       </c>
       <c r="D93">
-        <v>100322.987396249</v>
+        <v>100323.1493622969</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1696,13 +1696,13 @@
         <v>38139.31944444445</v>
       </c>
       <c r="B94">
-        <v>289.4564479933621</v>
+        <v>289.3235698820113</v>
       </c>
       <c r="C94">
-        <v>0.01003865005725558</v>
+        <v>0.01003433949986425</v>
       </c>
       <c r="D94">
-        <v>100322.7680843718</v>
+        <v>100322.8849801048</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1710,13 +1710,13 @@
         <v>38139.32291666666</v>
       </c>
       <c r="B95">
-        <v>289.2496088887537</v>
+        <v>288.9358362949198</v>
       </c>
       <c r="C95">
-        <v>0.0100490749818583</v>
+        <v>0.01002490686551499</v>
       </c>
       <c r="D95">
-        <v>100322.7601000589</v>
+        <v>100322.9543554879</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1724,13 +1724,13 @@
         <v>38139.32638888889</v>
       </c>
       <c r="B96">
-        <v>289.8042074198721</v>
+        <v>289.6200060153054</v>
       </c>
       <c r="C96">
-        <v>0.01008264677637174</v>
+        <v>0.01007047426724478</v>
       </c>
       <c r="D96">
-        <v>100322.5304173134</v>
+        <v>100322.6873687964</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1738,13 +1738,13 @@
         <v>38139.32986111111</v>
       </c>
       <c r="B97">
-        <v>289.6115469842892</v>
+        <v>289.2478261582143</v>
       </c>
       <c r="C97">
-        <v>0.01009938315134001</v>
+        <v>0.01006550705730791</v>
       </c>
       <c r="D97">
-        <v>100322.5044324658</v>
+        <v>100322.7367829183</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1752,13 +1752,13 @@
         <v>38139.33333333334</v>
       </c>
       <c r="B98">
-        <v>290.169992500127</v>
+        <v>289.9303526449244</v>
       </c>
       <c r="C98">
-        <v>0.0101545604121369</v>
+        <v>0.01013874088950144</v>
       </c>
       <c r="D98">
-        <v>100322.2683688609</v>
+        <v>100322.4657728258</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1766,13 +1766,13 @@
         <v>38139.33680555555</v>
       </c>
       <c r="B99">
-        <v>290.0171108159876</v>
+        <v>289.6026599742266</v>
       </c>
       <c r="C99">
-        <v>0.01017339237362375</v>
+        <v>0.01013177311666926</v>
       </c>
       <c r="D99">
-        <v>100322.1309915165</v>
+        <v>100322.4012423183</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1780,13 +1780,13 @@
         <v>38139.34027777778</v>
       </c>
       <c r="B100">
-        <v>290.6115261796544</v>
+        <v>290.3086661092045</v>
       </c>
       <c r="C100">
-        <v>0.01022847549314649</v>
+        <v>0.01020607640162769</v>
       </c>
       <c r="D100">
-        <v>100321.7625371415</v>
+        <v>100322.0049892651</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1794,13 +1794,13 @@
         <v>38139.34375</v>
       </c>
       <c r="B101">
-        <v>290.5070372900633</v>
+        <v>290.0313542404858</v>
       </c>
       <c r="C101">
-        <v>0.01024202565270632</v>
+        <v>0.0101889804666332</v>
       </c>
       <c r="D101">
-        <v>100321.56748296</v>
+        <v>100321.8846840237</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1808,13 +1808,13 @@
         <v>38139.34722222222</v>
       </c>
       <c r="B102">
-        <v>291.0827165944457</v>
+        <v>290.7049615727925</v>
       </c>
       <c r="C102">
-        <v>0.01029497166477962</v>
+        <v>0.01026568810379086</v>
       </c>
       <c r="D102">
-        <v>100321.2008101959</v>
+        <v>100321.4968490918</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1822,13 +1822,13 @@
         <v>38139.35069444445</v>
       </c>
       <c r="B103">
-        <v>291.006483564766</v>
+        <v>290.4618847831899</v>
       </c>
       <c r="C103">
-        <v>0.010278039400608</v>
+        <v>0.01019566891599104</v>
       </c>
       <c r="D103">
-        <v>100320.9980797433</v>
+        <v>100321.3663732509</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1836,13 +1836,13 @@
         <v>38139.35416666666</v>
       </c>
       <c r="B104">
-        <v>291.5477932033751</v>
+        <v>291.0899417639715</v>
       </c>
       <c r="C104">
-        <v>0.01033732397069995</v>
+        <v>0.01028844599968149</v>
       </c>
       <c r="D104">
-        <v>100320.6390903357</v>
+        <v>100320.9929652767</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1850,13 +1850,13 @@
         <v>38139.35763888889</v>
       </c>
       <c r="B105">
-        <v>291.5112526091729</v>
+        <v>290.88607264477</v>
       </c>
       <c r="C105">
-        <v>0.01032709097272927</v>
+        <v>0.01023580972341641</v>
       </c>
       <c r="D105">
-        <v>100320.4202769092</v>
+        <v>100320.845891508</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1864,13 +1864,13 @@
         <v>38139.36111111111</v>
       </c>
       <c r="B106">
-        <v>292.0184137174307</v>
+        <v>291.4710480104781</v>
       </c>
       <c r="C106">
-        <v>0.01039351486602612</v>
+        <v>0.01033713840349622</v>
       </c>
       <c r="D106">
-        <v>100320.0686871912</v>
+        <v>100320.4845623471</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1878,13 +1878,13 @@
         <v>38139.36458333334</v>
       </c>
       <c r="B107">
-        <v>292.0328243322114</v>
+        <v>291.3164686446555</v>
       </c>
       <c r="C107">
-        <v>0.0103766235167104</v>
+        <v>0.01029195118037491</v>
       </c>
       <c r="D107">
-        <v>100319.8323407454</v>
+        <v>100320.3194218037</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1892,13 +1892,13 @@
         <v>38139.36805555555</v>
       </c>
       <c r="B108">
-        <v>292.5068661882279</v>
+        <v>291.8631068741261</v>
       </c>
       <c r="C108">
-        <v>0.01045162663595046</v>
+        <v>0.01039786424597066</v>
       </c>
       <c r="D108">
-        <v>100319.4869330982</v>
+        <v>100319.9674145514</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1906,13 +1906,13 @@
         <v>38139.37152777778</v>
       </c>
       <c r="B109">
-        <v>292.5697063245166</v>
+        <v>291.7583274622341</v>
       </c>
       <c r="C109">
-        <v>0.01041563235494503</v>
+        <v>0.01035703004598732</v>
       </c>
       <c r="D109">
-        <v>100319.2357194072</v>
+        <v>100319.7853300749</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1920,13 +1920,13 @@
         <v>38139.375</v>
       </c>
       <c r="B110">
-        <v>293.0078186630792</v>
+        <v>292.2583020347475</v>
       </c>
       <c r="C110">
-        <v>0.01050494500392752</v>
+        <v>0.01046067524058366</v>
       </c>
       <c r="D110">
-        <v>100318.8978195652</v>
+        <v>100319.4471942852</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1934,13 +1934,13 @@
         <v>38139.37847222222</v>
       </c>
       <c r="B111">
-        <v>293.1221729287363</v>
+        <v>292.2108744631795</v>
       </c>
       <c r="C111">
-        <v>0.0104843217941468</v>
+        <v>0.01042992286451214</v>
       </c>
       <c r="D111">
-        <v>100318.6027527551</v>
+        <v>100319.216325069</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1948,13 +1948,13 @@
         <v>38139.38194444445</v>
       </c>
       <c r="B112">
-        <v>293.5694717520324</v>
+        <v>292.7251002832098</v>
       </c>
       <c r="C112">
-        <v>0.01057031875792516</v>
+        <v>0.01052619698015402</v>
       </c>
       <c r="D112">
-        <v>100318.1996190148</v>
+        <v>100318.8109131536</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1962,13 +1962,13 @@
         <v>38139.38541666666</v>
       </c>
       <c r="B113">
-        <v>293.7752862292701</v>
+        <v>292.7672561019655</v>
       </c>
       <c r="C113">
-        <v>0.01056700414234031</v>
+        <v>0.01051051111165801</v>
       </c>
       <c r="D113">
-        <v>100317.8339726854</v>
+        <v>100318.5108642279</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -1976,13 +1976,13 @@
         <v>38139.38888888889</v>
       </c>
       <c r="B114">
-        <v>294.196344144267</v>
+        <v>293.2454100695036</v>
       </c>
       <c r="C114">
-        <v>0.01066782587898908</v>
+        <v>0.01062257687183616</v>
       </c>
       <c r="D114">
-        <v>100317.4216598409</v>
+        <v>100318.1030900904</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1990,13 +1990,13 @@
         <v>38139.39236111111</v>
       </c>
       <c r="B115">
-        <v>294.446488166738</v>
+        <v>293.3324931416122</v>
       </c>
       <c r="C115">
-        <v>0.01067575417836434</v>
+        <v>0.01061704239820485</v>
       </c>
       <c r="D115">
-        <v>100317.0454235152</v>
+        <v>100317.7915755715</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2004,13 +2004,13 @@
         <v>38139.39583333334</v>
       </c>
       <c r="B116">
-        <v>294.8280280160432</v>
+        <v>293.7626612834375</v>
       </c>
       <c r="C116">
-        <v>0.01078152635939588</v>
+        <v>0.01073494196615412</v>
       </c>
       <c r="D116">
-        <v>100316.6422628471</v>
+        <v>100317.3966695108</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2018,13 +2018,13 @@
         <v>38139.39930555555</v>
       </c>
       <c r="B117">
-        <v>295.0901225048482</v>
+        <v>293.8703119007391</v>
       </c>
       <c r="C117">
-        <v>0.01076966488448573</v>
+        <v>0.01070915066117292</v>
       </c>
       <c r="D117">
-        <v>100316.2715138543</v>
+        <v>100317.0867706877</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2032,13 +2032,13 @@
         <v>38139.40277777778</v>
       </c>
       <c r="B118">
-        <v>295.4135169723676</v>
+        <v>294.2303117445761</v>
       </c>
       <c r="C118">
-        <v>0.01087004991857102</v>
+        <v>0.01082356830908392</v>
       </c>
       <c r="D118">
-        <v>100315.8936695493</v>
+        <v>100316.7209060396</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2046,13 +2046,13 @@
         <v>38139.40625</v>
       </c>
       <c r="B119">
-        <v>295.687388825527</v>
+        <v>294.3608192326724</v>
       </c>
       <c r="C119">
-        <v>0.01087107015432118</v>
+        <v>0.01080657230209874</v>
       </c>
       <c r="D119">
-        <v>100315.5272761717</v>
+        <v>100316.4106630228</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2060,13 +2060,13 @@
         <v>38139.40972222222</v>
       </c>
       <c r="B120">
-        <v>295.9855611435715</v>
+        <v>294.6842329002171</v>
       </c>
       <c r="C120">
-        <v>0.01093081851352831</v>
+        <v>0.01089863893990941</v>
       </c>
       <c r="D120">
-        <v>100315.1593503192</v>
+        <v>100316.0564103729</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2074,13 +2074,13 @@
         <v>38139.41319444445</v>
       </c>
       <c r="B121">
-        <v>296.2652227211436</v>
+        <v>294.8396259231457</v>
       </c>
       <c r="C121">
-        <v>0.01094757870145056</v>
+        <v>0.01089096673907123</v>
       </c>
       <c r="D121">
-        <v>100314.7959136904</v>
+        <v>100315.7423296554</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2088,13 +2088,13 @@
         <v>38139.41666666666</v>
       </c>
       <c r="B122">
-        <v>296.5547717346699</v>
+        <v>295.1297619537679</v>
       </c>
       <c r="C122">
-        <v>0.01098152876992604</v>
+        <v>0.01098515829362715</v>
       </c>
       <c r="D122">
-        <v>100314.4338261661</v>
+        <v>100315.3994624655</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2102,13 +2102,13 @@
         <v>38139.42013888889</v>
       </c>
       <c r="B123">
-        <v>296.786948042918</v>
+        <v>295.2632402163666</v>
       </c>
       <c r="C123">
-        <v>0.01099146830084846</v>
+        <v>0.0109555245385431</v>
       </c>
       <c r="D123">
-        <v>100314.1924882853</v>
+        <v>100315.2015536217</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2116,13 +2116,13 @@
         <v>38139.42361111111</v>
       </c>
       <c r="B124">
-        <v>296.9438010119737</v>
+        <v>295.4091675632997</v>
       </c>
       <c r="C124">
-        <v>0.01099346631728956</v>
+        <v>0.01100046222759435</v>
       </c>
       <c r="D124">
-        <v>100314.0544663774</v>
+        <v>100315.0812724422</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2130,13 +2130,13 @@
         <v>38139.42708333334</v>
       </c>
       <c r="B125">
-        <v>297.082455084514</v>
+        <v>295.4831569559095</v>
       </c>
       <c r="C125">
-        <v>0.01098174020095452</v>
+        <v>0.01094478517312657</v>
       </c>
       <c r="D125">
-        <v>100313.9431979186</v>
+        <v>100314.9954342097</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2144,13 +2144,13 @@
         <v>38139.43055555555</v>
       </c>
       <c r="B126">
-        <v>297.2177151916362</v>
+        <v>295.6109335790453</v>
       </c>
       <c r="C126">
-        <v>0.01096819323617299</v>
+        <v>0.01096847330403338</v>
       </c>
       <c r="D126">
-        <v>100313.8293100389</v>
+        <v>100314.8928007486</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2158,13 +2158,13 @@
         <v>38139.43402777778</v>
       </c>
       <c r="B127">
-        <v>297.361806685555</v>
+        <v>295.7072661129058</v>
       </c>
       <c r="C127">
-        <v>0.01094684449482355</v>
+        <v>0.01090508520958274</v>
       </c>
       <c r="D127">
-        <v>100313.7121244083</v>
+        <v>100314.7941520564</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2172,13 +2172,13 @@
         <v>38139.4375</v>
       </c>
       <c r="B128">
-        <v>297.4936896963714</v>
+        <v>295.8310148679575</v>
       </c>
       <c r="C128">
-        <v>0.01092487762287879</v>
+        <v>0.01092071468596244</v>
       </c>
       <c r="D128">
-        <v>100313.6032956213</v>
+        <v>100314.6943198738</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2186,13 +2186,13 @@
         <v>38139.44097222222</v>
       </c>
       <c r="B129">
-        <v>297.6191443755032</v>
+        <v>295.9206190758033</v>
       </c>
       <c r="C129">
-        <v>0.01090101923783126</v>
+        <v>0.01085556172966511</v>
       </c>
       <c r="D129">
-        <v>100313.5056759465</v>
+        <v>100314.6103348114</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2200,13 +2200,13 @@
         <v>38139.44444444445</v>
       </c>
       <c r="B130">
-        <v>297.7254138239911</v>
+        <v>296.0193385298675</v>
       </c>
       <c r="C130">
-        <v>0.01087618987715932</v>
+        <v>0.01086357511246781</v>
       </c>
       <c r="D130">
-        <v>100313.4200770089</v>
+        <v>100314.5312976446</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2214,13 +2214,13 @@
         <v>38139.44791666666</v>
       </c>
       <c r="B131">
-        <v>297.8304314105725</v>
+        <v>296.0977019355593</v>
       </c>
       <c r="C131">
-        <v>0.01084767964103598</v>
+        <v>0.01079547062947006</v>
       </c>
       <c r="D131">
-        <v>100313.3392360016</v>
+        <v>100314.4597863367</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2228,13 +2228,13 @@
         <v>38139.45138888889</v>
       </c>
       <c r="B132">
-        <v>297.9192407221078</v>
+        <v>296.1806938765091</v>
       </c>
       <c r="C132">
-        <v>0.01081894636014739</v>
+        <v>0.0107943100728684</v>
       </c>
       <c r="D132">
-        <v>100313.2669190424</v>
+        <v>100314.391299648</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2242,13 +2242,13 @@
         <v>38139.45486111111</v>
       </c>
       <c r="B133">
-        <v>298.0052309537687</v>
+        <v>296.2517482977781</v>
       </c>
       <c r="C133">
-        <v>0.01079006950301456</v>
+        <v>0.01072928984858671</v>
       </c>
       <c r="D133">
-        <v>100313.1990425701</v>
+        <v>100314.3273953098</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2256,13 +2256,13 @@
         <v>38139.45833333334</v>
       </c>
       <c r="B134">
-        <v>298.0770649815195</v>
+        <v>296.3246275130018</v>
       </c>
       <c r="C134">
-        <v>0.01076023237555529</v>
+        <v>0.01071061191184831</v>
       </c>
       <c r="D134">
-        <v>100313.1390038026</v>
+        <v>100314.2667545069</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2270,13 +2270,13 @@
         <v>38139.46180555555</v>
       </c>
       <c r="B135">
-        <v>298.1927311643631</v>
+        <v>296.431190949737</v>
       </c>
       <c r="C135">
-        <v>0.01073399257191853</v>
+        <v>0.01065872790518067</v>
       </c>
       <c r="D135">
-        <v>100312.9703061219</v>
+        <v>100314.0984030987</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2284,13 +2284,13 @@
         <v>38139.46527777778</v>
       </c>
       <c r="B136">
-        <v>298.3630360282933</v>
+        <v>296.5960508424649</v>
       </c>
       <c r="C136">
-        <v>0.01072105939305998</v>
+        <v>0.01063566455656891</v>
       </c>
       <c r="D136">
-        <v>100312.7316846337</v>
+        <v>100313.8623753748</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2298,13 +2298,13 @@
         <v>38139.46875</v>
       </c>
       <c r="B137">
-        <v>298.5512839734304</v>
+        <v>296.7673069059034</v>
       </c>
       <c r="C137">
-        <v>0.0107107841028328</v>
+        <v>0.0106128125523536</v>
       </c>
       <c r="D137">
-        <v>100312.4725374488</v>
+        <v>100313.6107552398</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2312,13 +2312,13 @@
         <v>38139.47222222222</v>
       </c>
       <c r="B138">
-        <v>298.7501852961416</v>
+        <v>296.9479590443291</v>
       </c>
       <c r="C138">
-        <v>0.01070890820536266</v>
+        <v>0.01060587690619528</v>
       </c>
       <c r="D138">
-        <v>100312.2135564701</v>
+        <v>100313.3613798265</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2326,13 +2326,13 @@
         <v>38139.47569444445</v>
       </c>
       <c r="B139">
-        <v>298.9433461772317</v>
+        <v>297.1155660640779</v>
       </c>
       <c r="C139">
-        <v>0.01073152025395</v>
+        <v>0.0106219727504659</v>
       </c>
       <c r="D139">
-        <v>100311.9557660126</v>
+        <v>100313.1152295227</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2340,13 +2340,13 @@
         <v>38139.47916666666</v>
       </c>
       <c r="B140">
-        <v>299.1452708008266</v>
+        <v>297.2963643308066</v>
       </c>
       <c r="C140">
-        <v>0.01075611313438089</v>
+        <v>0.01064461377565002</v>
       </c>
       <c r="D140">
-        <v>100311.6924301106</v>
+        <v>100312.8630287973</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2354,13 +2354,13 @@
         <v>38139.48263888889</v>
       </c>
       <c r="B141">
-        <v>299.3347494248559</v>
+        <v>297.4596689922862</v>
       </c>
       <c r="C141">
-        <v>0.01076894740248404</v>
+        <v>0.01065399197104675</v>
       </c>
       <c r="D141">
-        <v>100311.4354780309</v>
+        <v>100312.6185595177</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2368,13 +2368,13 @@
         <v>38139.48611111111</v>
       </c>
       <c r="B142">
-        <v>299.5232641464618</v>
+        <v>297.6258455847349</v>
       </c>
       <c r="C142">
-        <v>0.01077898601183498</v>
+        <v>0.01066362475610683</v>
       </c>
       <c r="D142">
-        <v>100311.1812517118</v>
+        <v>100312.3759625866</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2382,13 +2382,13 @@
         <v>38139.48958333334</v>
       </c>
       <c r="B143">
-        <v>299.7055478788269</v>
+        <v>297.7806537712223</v>
       </c>
       <c r="C143">
-        <v>0.01078054959976457</v>
+        <v>0.01066384602407794</v>
       </c>
       <c r="D143">
-        <v>100310.9291452345</v>
+        <v>100312.1365481908</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2396,13 +2396,13 @@
         <v>38139.49305555555</v>
       </c>
       <c r="B144">
-        <v>299.8874861438472</v>
+        <v>297.9401025163229</v>
       </c>
       <c r="C144">
-        <v>0.01078302812858528</v>
+        <v>0.01066664755628681</v>
       </c>
       <c r="D144">
-        <v>100310.678136618</v>
+        <v>100311.8968244819</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2410,13 +2410,13 @@
         <v>38139.49652777778</v>
       </c>
       <c r="B145">
-        <v>300.0632050829231</v>
+        <v>298.0903201507275</v>
       </c>
       <c r="C145">
-        <v>0.01078244252805525</v>
+        <v>0.01066316852230699</v>
       </c>
       <c r="D145">
-        <v>100310.4295589356</v>
+        <v>100311.6600978031</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2424,13 +2424,13 @@
         <v>38139.5</v>
       </c>
       <c r="B146">
-        <v>300.2388364790723</v>
+        <v>298.2441137803126</v>
       </c>
       <c r="C146">
-        <v>0.01078267686737409</v>
+        <v>0.01066278166477631</v>
       </c>
       <c r="D146">
-        <v>100310.1825397484</v>
+        <v>100311.4236953061</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2438,13 +2438,13 @@
         <v>38139.50347222222</v>
       </c>
       <c r="B147">
-        <v>300.3895475561341</v>
+        <v>298.3734238740144</v>
       </c>
       <c r="C147">
-        <v>0.01078026572425615</v>
+        <v>0.01065915436005577</v>
       </c>
       <c r="D147">
-        <v>100309.9516670369</v>
+        <v>100311.2030039872</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2452,13 +2452,13 @@
         <v>38139.50694444445</v>
       </c>
       <c r="B148">
-        <v>300.5324962883458</v>
+        <v>298.4982336279342</v>
       </c>
       <c r="C148">
-        <v>0.01078127766807668</v>
+        <v>0.01066094781966294</v>
       </c>
       <c r="D148">
-        <v>100309.7269610767</v>
+        <v>100310.9874628823</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2466,13 +2466,13 @@
         <v>38139.51041666666</v>
       </c>
       <c r="B149">
-        <v>300.6680230398809</v>
+        <v>298.6171861252661</v>
       </c>
       <c r="C149">
-        <v>0.01077803537186577</v>
+        <v>0.0106582839117674</v>
       </c>
       <c r="D149">
-        <v>100309.5052584594</v>
+        <v>100310.773739488</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2480,13 +2480,13 @@
         <v>38139.51388888889</v>
       </c>
       <c r="B150">
-        <v>300.7989593042555</v>
+        <v>298.7353899773483</v>
       </c>
       <c r="C150">
-        <v>0.01077658007068786</v>
+        <v>0.01066071769659337</v>
       </c>
       <c r="D150">
-        <v>100309.2880517098</v>
+        <v>100310.5627479508</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2494,13 +2494,13 @@
         <v>38139.51736111111</v>
       </c>
       <c r="B151">
-        <v>300.9240448107224</v>
+        <v>298.8474586916374</v>
       </c>
       <c r="C151">
-        <v>0.01077542472520659</v>
+        <v>0.01065874984707655</v>
       </c>
       <c r="D151">
-        <v>100309.0747348313</v>
+        <v>100310.3556133026</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2508,13 +2508,13 @@
         <v>38139.52083333334</v>
       </c>
       <c r="B152">
-        <v>301.0450212927709</v>
+        <v>298.9580914286506</v>
       </c>
       <c r="C152">
-        <v>0.01077675559867011</v>
+        <v>0.01066112498448289</v>
       </c>
       <c r="D152">
-        <v>100308.8647853295</v>
+        <v>100310.151003209</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2522,13 +2522,13 @@
         <v>38139.52430555555</v>
       </c>
       <c r="B153">
-        <v>301.1510283473275</v>
+        <v>299.0538779029598</v>
       </c>
       <c r="C153">
-        <v>0.01077727993349061</v>
+        <v>0.01065910335743008</v>
       </c>
       <c r="D153">
-        <v>100308.6661589004</v>
+        <v>100309.9572322062</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2536,13 +2536,13 @@
         <v>38139.52777777778</v>
       </c>
       <c r="B154">
-        <v>301.2472986307649</v>
+        <v>299.141691526435</v>
       </c>
       <c r="C154">
-        <v>0.01077919498670389</v>
+        <v>0.01065949284344392</v>
       </c>
       <c r="D154">
-        <v>100308.4752271585</v>
+        <v>100309.7704082885</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2550,13 +2550,13 @@
         <v>38139.53125</v>
       </c>
       <c r="B155">
-        <v>301.3349592842347</v>
+        <v>299.222165099981</v>
       </c>
       <c r="C155">
-        <v>0.01075138134922328</v>
+        <v>0.01062753532900422</v>
       </c>
       <c r="D155">
-        <v>100308.2890565176</v>
+        <v>100309.587344188</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2564,13 +2564,13 @@
         <v>38139.53472222222</v>
       </c>
       <c r="B156">
-        <v>301.4177611073493</v>
+        <v>299.3002095011351</v>
       </c>
       <c r="C156">
-        <v>0.01072793364369545</v>
+        <v>0.0106021614948111</v>
       </c>
       <c r="D156">
-        <v>100308.1067517994</v>
+        <v>100309.4068513846</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2578,13 +2578,13 @@
         <v>38139.53819444445</v>
       </c>
       <c r="B157">
-        <v>301.4917648463016</v>
+        <v>299.3728923318791</v>
       </c>
       <c r="C157">
-        <v>0.0107109755246212</v>
+        <v>0.01058268138866507</v>
       </c>
       <c r="D157">
-        <v>100307.9294319308</v>
+        <v>100309.2293374599</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2592,13 +2592,13 @@
         <v>38139.54166666666</v>
       </c>
       <c r="B158">
-        <v>301.5607402115924</v>
+        <v>299.4449137060875</v>
       </c>
       <c r="C158">
-        <v>0.01070216383909618</v>
+        <v>0.01057176172416927</v>
       </c>
       <c r="D158">
-        <v>100307.7559471394</v>
+        <v>100309.0539511512</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2606,13 +2606,13 @@
         <v>38139.54513888889</v>
       </c>
       <c r="B159">
-        <v>301.6045080060126</v>
+        <v>299.4909443304132</v>
       </c>
       <c r="C159">
-        <v>0.01071458209779984</v>
+        <v>0.01058192009068141</v>
       </c>
       <c r="D159">
-        <v>100307.6561031736</v>
+        <v>100308.9519424406</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2620,13 +2620,13 @@
         <v>38139.54861111111</v>
       </c>
       <c r="B160">
-        <v>301.7789843490049</v>
+        <v>299.6615405310637</v>
       </c>
       <c r="C160">
-        <v>0.01075962912062641</v>
+        <v>0.01062833875389805</v>
       </c>
       <c r="D160">
-        <v>100307.4449856817</v>
+        <v>100308.7435300586</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2634,13 +2634,13 @@
         <v>38139.55208333334</v>
       </c>
       <c r="B161">
-        <v>302.035180279814</v>
+        <v>299.8974729035555</v>
       </c>
       <c r="C161">
-        <v>0.01081491392867614</v>
+        <v>0.01068540636383665</v>
       </c>
       <c r="D161">
-        <v>100307.1515735931</v>
+        <v>100308.46355137</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2648,13 +2648,13 @@
         <v>38139.55555555555</v>
       </c>
       <c r="B162">
-        <v>302.3036600863389</v>
+        <v>300.1335542727609</v>
       </c>
       <c r="C162">
-        <v>0.01086074552396664</v>
+        <v>0.01073243110815231</v>
       </c>
       <c r="D162">
-        <v>100306.8553469006</v>
+        <v>100308.1880039049</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2662,13 +2662,13 @@
         <v>38139.55902777778</v>
       </c>
       <c r="B163">
-        <v>302.5107989864116</v>
+        <v>300.3089821830346</v>
       </c>
       <c r="C163">
-        <v>0.01090273481770702</v>
+        <v>0.01077428344737666</v>
       </c>
       <c r="D163">
-        <v>100306.5913787436</v>
+        <v>100307.9456763065</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2676,13 +2676,13 @@
         <v>38139.5625</v>
       </c>
       <c r="B164">
-        <v>302.6976661098455</v>
+        <v>300.4653198952013</v>
       </c>
       <c r="C164">
-        <v>0.01095637247062811</v>
+        <v>0.01082871475825073</v>
       </c>
       <c r="D164">
-        <v>100306.3477098067</v>
+        <v>100307.7221273813</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2690,13 +2690,13 @@
         <v>38139.56597222222</v>
       </c>
       <c r="B165">
-        <v>302.8241038647296</v>
+        <v>300.56913608832</v>
       </c>
       <c r="C165">
-        <v>0.01100475624727562</v>
+        <v>0.01087712683623527</v>
       </c>
       <c r="D165">
-        <v>100306.1386462849</v>
+        <v>100307.5304041254</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2704,13 +2704,13 @@
         <v>38139.56944444445</v>
       </c>
       <c r="B166">
-        <v>302.9274101898019</v>
+        <v>300.6547791205846</v>
       </c>
       <c r="C166">
-        <v>0.01105826111018019</v>
+        <v>0.01092942889480613</v>
       </c>
       <c r="D166">
-        <v>100305.952500119</v>
+        <v>100307.3588793124</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2718,13 +2718,13 @@
         <v>38139.57291666666</v>
       </c>
       <c r="B167">
-        <v>302.9857899966144</v>
+        <v>300.7057635710504</v>
       </c>
       <c r="C167">
-        <v>0.0111017298394408</v>
+        <v>0.01097396933273287</v>
       </c>
       <c r="D167">
-        <v>100305.7904063422</v>
+        <v>100307.2072434048</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2732,13 +2732,13 @@
         <v>38139.57638888889</v>
       </c>
       <c r="B168">
-        <v>303.0319074120004</v>
+        <v>300.7503715919754</v>
       </c>
       <c r="C168">
-        <v>0.01114734751095803</v>
+        <v>0.01102075987294378</v>
       </c>
       <c r="D168">
-        <v>100305.6440659369</v>
+        <v>100307.0677783541</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2746,13 +2746,13 @@
         <v>38139.57986111111</v>
       </c>
       <c r="B169">
-        <v>303.0460550190069</v>
+        <v>300.7705790272295</v>
       </c>
       <c r="C169">
-        <v>0.01118422718080339</v>
+        <v>0.01105752080735901</v>
       </c>
       <c r="D169">
-        <v>100305.5157829762</v>
+        <v>100306.9430966891</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2760,13 +2760,13 @@
         <v>38139.58333333334</v>
       </c>
       <c r="B170">
-        <v>303.0555381120228</v>
+        <v>300.7916235180638</v>
       </c>
       <c r="C170">
-        <v>0.01119247207099109</v>
+        <v>0.01106833551090974</v>
       </c>
       <c r="D170">
-        <v>100305.398594914</v>
+        <v>100306.8261202771</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2774,13 +2774,13 @@
         <v>38139.58680555555</v>
       </c>
       <c r="B171">
-        <v>302.9450090630891</v>
+        <v>300.6868413719258</v>
       </c>
       <c r="C171">
-        <v>0.01119192852909691</v>
+        <v>0.01106842085386955</v>
       </c>
       <c r="D171">
-        <v>100305.581260579</v>
+        <v>100307.015050422</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2788,13 +2788,13 @@
         <v>38139.59027777778</v>
       </c>
       <c r="B172">
-        <v>302.8199497260884</v>
+        <v>300.5701228312388</v>
       </c>
       <c r="C172">
-        <v>0.01120452757336822</v>
+        <v>0.01108221209909022</v>
       </c>
       <c r="D172">
-        <v>100305.8078152692</v>
+        <v>100307.2485404175</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2802,13 +2802,13 @@
         <v>38139.59375</v>
       </c>
       <c r="B173">
-        <v>302.6220570795794</v>
+        <v>300.3947389729344</v>
       </c>
       <c r="C173">
-        <v>0.01120772345080906</v>
+        <v>0.01108750760390635</v>
       </c>
       <c r="D173">
-        <v>100306.0507744137</v>
+        <v>100307.4947222341</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2816,13 +2816,13 @@
         <v>38139.59722222222</v>
       </c>
       <c r="B174">
-        <v>302.4213604561727</v>
+        <v>300.2237755536545</v>
       </c>
       <c r="C174">
-        <v>0.0112182191328816</v>
+        <v>0.01110020317276924</v>
       </c>
       <c r="D174">
-        <v>100306.2920491999</v>
+        <v>100307.7337248722</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2830,13 +2830,13 @@
         <v>38139.60069444445</v>
       </c>
       <c r="B175">
-        <v>302.1674702641635</v>
+        <v>300.0140429394452</v>
       </c>
       <c r="C175">
-        <v>0.01122040126565489</v>
+        <v>0.01110631673695059</v>
       </c>
       <c r="D175">
-        <v>100306.5518417263</v>
+        <v>100307.9846692181</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2844,13 +2844,13 @@
         <v>38139.60416666666</v>
       </c>
       <c r="B176">
-        <v>301.9316189064742</v>
+        <v>299.8254659686128</v>
       </c>
       <c r="C176">
-        <v>0.01123245703319797</v>
+        <v>0.0111204254279438</v>
       </c>
       <c r="D176">
-        <v>100306.8153791495</v>
+        <v>100308.2337604433</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2858,13 +2858,13 @@
         <v>38139.60763888889</v>
       </c>
       <c r="B177">
-        <v>301.7675036830868</v>
+        <v>299.7176870832135</v>
       </c>
       <c r="C177">
-        <v>0.01123783310951475</v>
+        <v>0.01112689744648416</v>
       </c>
       <c r="D177">
-        <v>100306.9851947991</v>
+        <v>100308.3838054721</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2872,13 +2872,13 @@
         <v>38139.61111111111</v>
       </c>
       <c r="B178">
-        <v>301.6818565445213</v>
+        <v>299.6784307813496</v>
       </c>
       <c r="C178">
-        <v>0.01125236508988438</v>
+        <v>0.01114546135395802</v>
       </c>
       <c r="D178">
-        <v>100307.1032015118</v>
+        <v>100308.4847547293</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2886,13 +2886,13 @@
         <v>38139.61458333334</v>
       </c>
       <c r="B179">
-        <v>301.5950623222889</v>
+        <v>299.6333771696796</v>
       </c>
       <c r="C179">
-        <v>0.01126097283079089</v>
+        <v>0.01115714452350006</v>
       </c>
       <c r="D179">
-        <v>100307.20635138</v>
+        <v>100308.5743311838</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -2900,13 +2900,13 @@
         <v>38139.61805555555</v>
       </c>
       <c r="B180">
-        <v>301.553694059439</v>
+        <v>299.6264370381111</v>
       </c>
       <c r="C180">
-        <v>0.01127877523539221</v>
+        <v>0.01118007187801216</v>
       </c>
       <c r="D180">
-        <v>100307.2878089223</v>
+        <v>100308.6435990531</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -2914,13 +2914,13 @@
         <v>38139.62152777778</v>
       </c>
       <c r="B181">
-        <v>301.4996997704497</v>
+        <v>299.6038972673197</v>
       </c>
       <c r="C181">
-        <v>0.01129143141432126</v>
+        <v>0.01119658317971481</v>
       </c>
       <c r="D181">
-        <v>100307.3589751134</v>
+        <v>100308.7056773967</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2928,13 +2928,13 @@
         <v>38139.625</v>
       </c>
       <c r="B182">
-        <v>301.48105213642</v>
+        <v>299.6115462455388</v>
       </c>
       <c r="C182">
-        <v>0.01131464110723856</v>
+        <v>0.01122248569768029</v>
       </c>
       <c r="D182">
-        <v>100307.4125684276</v>
+        <v>100308.7512022888</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -2942,13 +2942,13 @@
         <v>38139.62847222222</v>
       </c>
       <c r="B183">
-        <v>301.4598954681909</v>
+        <v>299.5959155020628</v>
       </c>
       <c r="C183">
-        <v>0.01131668413418605</v>
+        <v>0.01122839605087324</v>
       </c>
       <c r="D183">
-        <v>100307.3626790716</v>
+        <v>100308.7107746194</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2956,13 +2956,13 @@
         <v>38139.63194444445</v>
       </c>
       <c r="B184">
-        <v>301.3186622456141</v>
+        <v>299.470372006598</v>
       </c>
       <c r="C184">
-        <v>0.01130822342119913</v>
+        <v>0.01122356798677307</v>
       </c>
       <c r="D184">
-        <v>100307.45556969</v>
+        <v>100308.7986962677</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -2970,13 +2970,13 @@
         <v>38139.63541666666</v>
       </c>
       <c r="B185">
-        <v>301.2948659069655</v>
+        <v>299.4411252607812</v>
       </c>
       <c r="C185">
-        <v>0.01131021650342087</v>
+        <v>0.01122626977920102</v>
       </c>
       <c r="D185">
-        <v>100307.4854306065</v>
+        <v>100308.8275584821</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -2984,13 +2984,13 @@
         <v>38139.63888888889</v>
       </c>
       <c r="B186">
-        <v>301.3119953528923</v>
+        <v>299.4387819519548</v>
       </c>
       <c r="C186">
-        <v>0.01131138869942171</v>
+        <v>0.01124139799043355</v>
       </c>
       <c r="D186">
-        <v>100307.4544403643</v>
+        <v>100308.8105195352</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -2998,13 +2998,13 @@
         <v>38139.64236111111</v>
       </c>
       <c r="B187">
-        <v>301.3922964790783</v>
+        <v>299.4745635068833</v>
       </c>
       <c r="C187">
-        <v>0.01132448404566367</v>
+        <v>0.0112487548236179</v>
       </c>
       <c r="D187">
-        <v>100307.3905910086</v>
+        <v>100308.7734623876</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3012,13 +3012,13 @@
         <v>38139.64583333334</v>
       </c>
       <c r="B188">
-        <v>301.4183535941082</v>
+        <v>299.4565286769403</v>
       </c>
       <c r="C188">
-        <v>0.01133079018542195</v>
+        <v>0.01126333086381068</v>
       </c>
       <c r="D188">
-        <v>100307.3457414419</v>
+        <v>100308.7610724062</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3026,13 +3026,13 @@
         <v>38139.64930555555</v>
       </c>
       <c r="B189">
-        <v>301.3920520652299</v>
+        <v>299.3738442786135</v>
       </c>
       <c r="C189">
-        <v>0.01134649545272733</v>
+        <v>0.01126997542158376</v>
       </c>
       <c r="D189">
-        <v>100307.3799021615</v>
+        <v>100308.8302622766</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3040,13 +3040,13 @@
         <v>38139.65277777778</v>
       </c>
       <c r="B190">
-        <v>301.2789273062548</v>
+        <v>299.2194111620285</v>
       </c>
       <c r="C190">
-        <v>0.01135441955086166</v>
+        <v>0.01129817479017389</v>
       </c>
       <c r="D190">
-        <v>100307.4588343184</v>
+        <v>100308.9386583085</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3054,13 +3054,13 @@
         <v>38139.65625</v>
       </c>
       <c r="B191">
-        <v>301.1840056809855</v>
+        <v>299.0821825294997</v>
       </c>
       <c r="C191">
-        <v>0.0113696023700331</v>
+        <v>0.01131989564076308</v>
       </c>
       <c r="D191">
-        <v>100307.5402688528</v>
+        <v>100309.0444547748</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3068,13 +3068,13 @@
         <v>38139.65972222222</v>
       </c>
       <c r="B192">
-        <v>301.0349293303341</v>
+        <v>298.912535730427</v>
       </c>
       <c r="C192">
-        <v>0.01137727462469817</v>
+        <v>0.01134720311163046</v>
       </c>
       <c r="D192">
-        <v>100307.6373338707</v>
+        <v>100309.1605999321</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3082,13 +3082,13 @@
         <v>38139.66319444445</v>
       </c>
       <c r="B193">
-        <v>300.902336544231</v>
+        <v>298.7483532628196</v>
       </c>
       <c r="C193">
-        <v>0.01139356167569824</v>
+        <v>0.01137013370351334</v>
       </c>
       <c r="D193">
-        <v>100307.7362285409</v>
+        <v>100309.2772362071</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3096,13 +3096,13 @@
         <v>38139.66666666666</v>
       </c>
       <c r="B194">
-        <v>300.7256290268705</v>
+        <v>298.5669552528721</v>
       </c>
       <c r="C194">
-        <v>0.01140178695040084</v>
+        <v>0.01138994198854364</v>
       </c>
       <c r="D194">
-        <v>100307.846613307</v>
+        <v>100309.3981654023</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3110,13 +3110,13 @@
         <v>38139.67013888889</v>
       </c>
       <c r="B195">
-        <v>300.612292646918</v>
+        <v>298.4521037836366</v>
       </c>
       <c r="C195">
-        <v>0.01141910299526237</v>
+        <v>0.01141065940343539</v>
       </c>
       <c r="D195">
-        <v>100307.9589333128</v>
+        <v>100309.5029923685</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3124,13 +3124,13 @@
         <v>38139.67361111111</v>
       </c>
       <c r="B196">
-        <v>300.5118225735266</v>
+        <v>298.3734177215973</v>
       </c>
       <c r="C196">
-        <v>0.01143512159771402</v>
+        <v>0.01143124840586692</v>
       </c>
       <c r="D196">
-        <v>100308.0473850482</v>
+        <v>100309.5785368174</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3138,13 +3138,13 @@
         <v>38139.67708333334</v>
       </c>
       <c r="B197">
-        <v>300.422236214869</v>
+        <v>298.2859303022051</v>
       </c>
       <c r="C197">
-        <v>0.01148621400549158</v>
+        <v>0.01148105863034043</v>
       </c>
       <c r="D197">
-        <v>100308.1345337346</v>
+        <v>100309.656475182</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3152,13 +3152,13 @@
         <v>38139.68055555555</v>
       </c>
       <c r="B198">
-        <v>300.3119919217262</v>
+        <v>298.2057329059456</v>
       </c>
       <c r="C198">
-        <v>0.01154000719156477</v>
+        <v>0.01152780606606968</v>
       </c>
       <c r="D198">
-        <v>100308.2288511167</v>
+        <v>100309.7340124479</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3166,13 +3166,13 @@
         <v>38139.68402777778</v>
       </c>
       <c r="B199">
-        <v>300.2094156022042</v>
+        <v>298.1103412668802</v>
       </c>
       <c r="C199">
-        <v>0.01158900572862421</v>
+        <v>0.01156048386944378</v>
       </c>
       <c r="D199">
-        <v>100308.3249380751</v>
+        <v>100309.8164029133</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3180,13 +3180,13 @@
         <v>38139.6875</v>
       </c>
       <c r="B200">
-        <v>300.0950743147373</v>
+        <v>298.0312504485306</v>
       </c>
       <c r="C200">
-        <v>0.01163805254052314</v>
+        <v>0.01158786135508468</v>
       </c>
       <c r="D200">
-        <v>100308.4252422403</v>
+        <v>100309.8954490101</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3194,13 +3194,13 @@
         <v>38139.69097222222</v>
       </c>
       <c r="B201">
-        <v>299.9713706380384</v>
+        <v>297.9198511128716</v>
       </c>
       <c r="C201">
-        <v>0.01167436140635071</v>
+        <v>0.01160771958579546</v>
       </c>
       <c r="D201">
-        <v>100308.5455020266</v>
+        <v>100309.9987216741</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3208,13 +3208,13 @@
         <v>38139.69444444445</v>
       </c>
       <c r="B202">
-        <v>299.8380005545479</v>
+        <v>297.8228028731218</v>
       </c>
       <c r="C202">
-        <v>0.01170467932806942</v>
+        <v>0.01162882883472423</v>
       </c>
       <c r="D202">
-        <v>100308.6751242652</v>
+        <v>100310.1048697549</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3222,13 +3222,13 @@
         <v>38139.69791666666</v>
       </c>
       <c r="B203">
-        <v>299.700947601776</v>
+        <v>297.7001544840781</v>
       </c>
       <c r="C203">
-        <v>0.01172822017521898</v>
+        <v>0.01164479005719291</v>
       </c>
       <c r="D203">
-        <v>100308.8100587938</v>
+        <v>100310.2207822635</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3236,13 +3236,13 @@
         <v>38139.70138888889</v>
       </c>
       <c r="B204">
-        <v>299.5591511796123</v>
+        <v>297.6010655619418</v>
       </c>
       <c r="C204">
-        <v>0.0117494302803501</v>
+        <v>0.01166077271634077</v>
       </c>
       <c r="D204">
-        <v>100308.9502479951</v>
+        <v>100310.3343022874</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3250,13 +3250,13 @@
         <v>38139.70486111111</v>
       </c>
       <c r="B205">
-        <v>299.4113806672973</v>
+        <v>297.4703581157105</v>
       </c>
       <c r="C205">
-        <v>0.01176829641921825</v>
+        <v>0.0116744480229786</v>
       </c>
       <c r="D205">
-        <v>100309.0966561504</v>
+        <v>100310.4597249489</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3264,13 +3264,13 @@
         <v>38139.70833333334</v>
       </c>
       <c r="B206">
-        <v>299.261971229309</v>
+        <v>297.3644344310143</v>
       </c>
       <c r="C206">
-        <v>0.01178576486324802</v>
+        <v>0.01168884400950252</v>
       </c>
       <c r="D206">
-        <v>100309.2479193519</v>
+        <v>100310.5830535856</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3278,13 +3278,13 @@
         <v>38139.71180555555</v>
       </c>
       <c r="B207">
-        <v>299.1888893726986</v>
+        <v>297.3033043851274</v>
       </c>
       <c r="C207">
-        <v>0.01173316001980525</v>
+        <v>0.01164604971027973</v>
       </c>
       <c r="D207">
-        <v>100309.0577365857</v>
+        <v>100310.3784830006</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3292,13 +3292,13 @@
         <v>38139.71527777778</v>
       </c>
       <c r="B208">
-        <v>299.0007458970065</v>
+        <v>297.12674924373</v>
       </c>
       <c r="C208">
-        <v>0.01171033107906327</v>
+        <v>0.01162775545639314</v>
       </c>
       <c r="D208">
-        <v>100309.2953655551</v>
+        <v>100310.6041602901</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3306,13 +3306,13 @@
         <v>38139.71875</v>
       </c>
       <c r="B209">
-        <v>298.7742835551653</v>
+        <v>296.9126066666124</v>
       </c>
       <c r="C209">
-        <v>0.01169831917604227</v>
+        <v>0.01161609121882308</v>
       </c>
       <c r="D209">
-        <v>100309.6668721124</v>
+        <v>100310.9543312426</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3320,13 +3320,13 @@
         <v>38139.72222222222</v>
       </c>
       <c r="B210">
-        <v>298.5081372920435</v>
+        <v>296.689993006712</v>
       </c>
       <c r="C210">
-        <v>0.01168698700520939</v>
+        <v>0.0116049540481208</v>
       </c>
       <c r="D210">
-        <v>100310.0699459928</v>
+        <v>100311.3254204959</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3334,13 +3334,13 @@
         <v>38139.72569444445</v>
       </c>
       <c r="B211">
-        <v>298.2409900004354</v>
+        <v>296.4481771397889</v>
       </c>
       <c r="C211">
-        <v>0.01167730967156647</v>
+        <v>0.01159321084224963</v>
       </c>
       <c r="D211">
-        <v>100310.4597468188</v>
+        <v>100311.6877987905</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3348,13 +3348,13 @@
         <v>38139.72916666666</v>
       </c>
       <c r="B212">
-        <v>298.000674442484</v>
+        <v>296.2628580901679</v>
       </c>
       <c r="C212">
-        <v>0.01166373807070809</v>
+        <v>0.01158096007802826</v>
       </c>
       <c r="D212">
-        <v>100310.8315505247</v>
+        <v>100312.0239796739</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3362,13 +3362,13 @@
         <v>38139.73263888889</v>
       </c>
       <c r="B213">
-        <v>297.742172904462</v>
+        <v>296.0306495876056</v>
       </c>
       <c r="C213">
-        <v>0.01165065697028631</v>
+        <v>0.01156835396843023</v>
       </c>
       <c r="D213">
-        <v>100311.2464179827</v>
+        <v>100312.4098397849</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3376,13 +3376,13 @@
         <v>38139.73611111111</v>
       </c>
       <c r="B214">
-        <v>297.4516200057828</v>
+        <v>295.7981005210946</v>
       </c>
       <c r="C214">
-        <v>0.01163605315962878</v>
+        <v>0.01155334627817025</v>
       </c>
       <c r="D214">
-        <v>100311.6916627023</v>
+        <v>100312.8179890426</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3390,13 +3390,13 @@
         <v>38139.73958333334</v>
       </c>
       <c r="B215">
-        <v>297.1527984112778</v>
+        <v>295.5350219107301</v>
       </c>
       <c r="C215">
-        <v>0.01162100309474659</v>
+        <v>0.01153705553028067</v>
       </c>
       <c r="D215">
-        <v>100312.1492143976</v>
+        <v>100313.2418696153</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3404,13 +3404,13 @@
         <v>38139.74305555555</v>
       </c>
       <c r="B216">
-        <v>296.8308803933344</v>
+        <v>295.2786767489348</v>
       </c>
       <c r="C216">
-        <v>0.01160453828940713</v>
+        <v>0.01151965274233179</v>
       </c>
       <c r="D216">
-        <v>100312.6212015968</v>
+        <v>100313.6714199705</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3418,13 +3418,13 @@
         <v>38139.74652777778</v>
       </c>
       <c r="B217">
-        <v>296.4933511692155</v>
+        <v>294.9840338167355</v>
       </c>
       <c r="C217">
-        <v>0.01158517636580808</v>
+        <v>0.01150079484645062</v>
       </c>
       <c r="D217">
-        <v>100313.1070040707</v>
+        <v>100314.1176051081</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3432,13 +3432,13 @@
         <v>38139.75</v>
       </c>
       <c r="B218">
-        <v>296.1090782248982</v>
+        <v>294.6801922769337</v>
       </c>
       <c r="C218">
-        <v>0.01153436359457239</v>
+        <v>0.01144882489953396</v>
       </c>
       <c r="D218">
-        <v>100313.6181020344</v>
+        <v>100314.5770547146</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3446,13 +3446,13 @@
         <v>38139.75347222222</v>
       </c>
       <c r="B219">
-        <v>295.7687093000155</v>
+        <v>294.3927833067777</v>
       </c>
       <c r="C219">
-        <v>0.01148692269145097</v>
+        <v>0.01140170291425978</v>
       </c>
       <c r="D219">
-        <v>100313.9223862846</v>
+        <v>100314.8337626451</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3460,13 +3460,13 @@
         <v>38139.75694444445</v>
       </c>
       <c r="B220">
-        <v>295.4753037592018</v>
+        <v>294.1780150725273</v>
       </c>
       <c r="C220">
-        <v>0.01145230171275392</v>
+        <v>0.01136943309932281</v>
       </c>
       <c r="D220">
-        <v>100314.1387667906</v>
+        <v>100314.9993043999</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3474,13 +3474,13 @@
         <v>38139.76041666666</v>
       </c>
       <c r="B221">
-        <v>295.1746634050962</v>
+        <v>293.921139146833</v>
       </c>
       <c r="C221">
-        <v>0.01139635398178987</v>
+        <v>0.01131434112696452</v>
       </c>
       <c r="D221">
-        <v>100314.3430652606</v>
+        <v>100315.1638799039</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3488,13 +3488,13 @@
         <v>38139.76388888889</v>
       </c>
       <c r="B222">
-        <v>294.8665442852285</v>
+        <v>293.6882753996192</v>
       </c>
       <c r="C222">
-        <v>0.01134989222957528</v>
+        <v>0.01127082515030586</v>
       </c>
       <c r="D222">
-        <v>100314.5565747995</v>
+        <v>100315.3270513734</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3502,13 +3502,13 @@
         <v>38139.76736111111</v>
       </c>
       <c r="B223">
-        <v>294.5192720041217</v>
+        <v>293.3919182678835</v>
       </c>
       <c r="C223">
-        <v>0.01128325220639227</v>
+        <v>0.01120655585256511</v>
       </c>
       <c r="D223">
-        <v>100314.7810331445</v>
+        <v>100315.5054174405</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3516,13 +3516,13 @@
         <v>38139.77083333334</v>
       </c>
       <c r="B224">
-        <v>294.1708521172494</v>
+        <v>293.1308130682262</v>
       </c>
       <c r="C224">
-        <v>0.01122998751238568</v>
+        <v>0.011158122757042</v>
       </c>
       <c r="D224">
-        <v>100315.0001057911</v>
+        <v>100315.6656857315</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3530,13 +3530,13 @@
         <v>38139.77430555555</v>
       </c>
       <c r="B225">
-        <v>293.8486634324458</v>
+        <v>292.8669083223961</v>
       </c>
       <c r="C225">
-        <v>0.01115790762073338</v>
+        <v>0.01108923286897416</v>
       </c>
       <c r="D225">
-        <v>100315.1818955984</v>
+        <v>100315.7971761512</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3544,13 +3544,13 @@
         <v>38139.77777777778</v>
       </c>
       <c r="B226">
-        <v>293.5575569917095</v>
+        <v>292.6649548536976</v>
       </c>
       <c r="C226">
-        <v>0.01110687623121051</v>
+        <v>0.01104539600332946</v>
       </c>
       <c r="D226">
-        <v>100315.3357904237</v>
+        <v>100315.8919660617</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3558,13 +3558,13 @@
         <v>38139.78125</v>
       </c>
       <c r="B227">
-        <v>293.2600505512814</v>
+        <v>292.4268835629986</v>
       </c>
       <c r="C227">
-        <v>0.01103578230750259</v>
+        <v>0.01097780209099385</v>
       </c>
       <c r="D227">
-        <v>100315.47925371</v>
+        <v>100315.9866824525</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3572,13 +3572,13 @@
         <v>38139.78472222222</v>
       </c>
       <c r="B228">
-        <v>292.9769597388625</v>
+        <v>292.2740718907218</v>
       </c>
       <c r="C228">
-        <v>0.01099105206331525</v>
+        <v>0.01094446715082084</v>
       </c>
       <c r="D228">
-        <v>100315.6064734722</v>
+        <v>100316.0297273537</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3586,13 +3586,13 @@
         <v>38139.78819444445</v>
       </c>
       <c r="B229">
-        <v>292.6933194865246</v>
+        <v>292.2057296604419</v>
       </c>
       <c r="C229">
-        <v>0.01092425925086301</v>
+        <v>0.01089600198468155</v>
       </c>
       <c r="D229">
-        <v>100315.7191318875</v>
+        <v>100316.0036334277</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3600,13 +3600,13 @@
         <v>38139.79166666666</v>
       </c>
       <c r="B230">
-        <v>292.5727313766057</v>
+        <v>292.2380217172827</v>
       </c>
       <c r="C230">
-        <v>0.0108991909459768</v>
+        <v>0.01088629823704502</v>
       </c>
       <c r="D230">
-        <v>100315.7226501579</v>
+        <v>100315.9235473581</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3614,13 +3614,13 @@
         <v>38139.79513888889</v>
       </c>
       <c r="B231">
-        <v>292.5613486323468</v>
+        <v>292.2281818056295</v>
       </c>
       <c r="C231">
-        <v>0.01091427617644969</v>
+        <v>0.01090531717694057</v>
       </c>
       <c r="D231">
-        <v>100315.675501973</v>
+        <v>100315.8650481286</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3628,13 +3628,13 @@
         <v>38139.79861111111</v>
       </c>
       <c r="B232">
-        <v>292.5821966339134</v>
+        <v>292.2518991666058</v>
       </c>
       <c r="C232">
-        <v>0.01090220136266583</v>
+        <v>0.01089687682548298</v>
       </c>
       <c r="D232">
-        <v>100315.6074225703</v>
+        <v>100315.7970386728</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3642,13 +3642,13 @@
         <v>38139.80208333334</v>
       </c>
       <c r="B233">
-        <v>292.5582621266577</v>
+        <v>292.2097719435784</v>
       </c>
       <c r="C233">
-        <v>0.01091013356478618</v>
+        <v>0.01090380474872129</v>
       </c>
       <c r="D233">
-        <v>100315.5531586126</v>
+        <v>100315.7504454272</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3656,13 +3656,13 @@
         <v>38139.80555555555</v>
       </c>
       <c r="B234">
-        <v>292.5407156169052</v>
+        <v>292.206378873811</v>
       </c>
       <c r="C234">
-        <v>0.01093239900348645</v>
+        <v>0.01092557586933305</v>
       </c>
       <c r="D234">
-        <v>100315.5003133091</v>
+        <v>100315.6933242308</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3670,13 +3670,13 @@
         <v>38139.80902777778</v>
       </c>
       <c r="B235">
-        <v>292.4913329792997</v>
+        <v>292.1489587726833</v>
       </c>
       <c r="C235">
-        <v>0.01091807651003438</v>
+        <v>0.01091234153225053</v>
       </c>
       <c r="D235">
-        <v>100315.4583787022</v>
+        <v>100315.652893199</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3684,13 +3684,13 @@
         <v>38139.8125</v>
       </c>
       <c r="B236">
-        <v>292.4529129603266</v>
+        <v>292.1296616289843</v>
       </c>
       <c r="C236">
-        <v>0.01091781930669535</v>
+        <v>0.01091207360962514</v>
       </c>
       <c r="D236">
-        <v>100315.4280128582</v>
+        <v>100315.6153787827</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3698,13 +3698,13 @@
         <v>38139.81597222222</v>
       </c>
       <c r="B237">
-        <v>292.3508419432993</v>
+        <v>292.0306127404955</v>
       </c>
       <c r="C237">
-        <v>0.0109276192566509</v>
+        <v>0.01092113929277115</v>
       </c>
       <c r="D237">
-        <v>100315.4442890492</v>
+        <v>100315.6260422904</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3712,13 +3712,13 @@
         <v>38139.81944444445</v>
       </c>
       <c r="B238">
-        <v>292.3919006803362</v>
+        <v>292.0819048208453</v>
       </c>
       <c r="C238">
-        <v>0.01094810241439113</v>
+        <v>0.01094161529739567</v>
       </c>
       <c r="D238">
-        <v>100315.4079026034</v>
+        <v>100315.5838519151</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3726,13 +3726,13 @@
         <v>38139.82291666666</v>
       </c>
       <c r="B239">
-        <v>292.3400417371333</v>
+        <v>292.0240044509291</v>
       </c>
       <c r="C239">
-        <v>0.01092796003084434</v>
+        <v>0.01092335471276787</v>
       </c>
       <c r="D239">
-        <v>100315.3934944282</v>
+        <v>100315.5703429904</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3740,13 +3740,13 @@
         <v>38139.82638888889</v>
       </c>
       <c r="B240">
-        <v>292.3666815801043</v>
+        <v>292.0615629058377</v>
       </c>
       <c r="C240">
-        <v>0.01092243973419901</v>
+        <v>0.01091791455852084</v>
       </c>
       <c r="D240">
-        <v>100315.3586036439</v>
+        <v>100315.5319547898</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3754,13 +3754,13 @@
         <v>38139.82986111111</v>
       </c>
       <c r="B241">
-        <v>292.3024667210934</v>
+        <v>291.9897418121585</v>
       </c>
       <c r="C241">
-        <v>0.01092541939035988</v>
+        <v>0.01092039757111611</v>
       </c>
       <c r="D241">
-        <v>100315.3566677236</v>
+        <v>100315.531908089</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3768,13 +3768,13 @@
         <v>38139.83333333334</v>
       </c>
       <c r="B242">
-        <v>292.2971208378784</v>
+        <v>291.9986082046653</v>
       </c>
       <c r="C242">
-        <v>0.0108966361954766</v>
+        <v>0.01089373895604044</v>
       </c>
       <c r="D242">
-        <v>100315.344962603</v>
+        <v>100315.5153594543</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -3782,13 +3782,13 @@
         <v>38139.83680555555</v>
       </c>
       <c r="B243">
-        <v>292.2035404497091</v>
+        <v>291.8979009303565</v>
       </c>
       <c r="C243">
-        <v>0.01087785834868542</v>
+        <v>0.0108744965927503</v>
       </c>
       <c r="D243">
-        <v>100315.3941832614</v>
+        <v>100315.5661373303</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -3796,13 +3796,13 @@
         <v>38139.84027777778</v>
       </c>
       <c r="B244">
-        <v>292.1520695398203</v>
+        <v>291.8639009647915</v>
       </c>
       <c r="C244">
-        <v>0.01087463330727157</v>
+        <v>0.01087060115523784</v>
       </c>
       <c r="D244">
-        <v>100315.4359662336</v>
+        <v>100315.6013467435</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -3810,13 +3810,13 @@
         <v>38139.84375</v>
       </c>
       <c r="B245">
-        <v>292.0601306889612</v>
+        <v>291.7654874232646</v>
       </c>
       <c r="C245">
-        <v>0.01088115954970031</v>
+        <v>0.0108761631539578</v>
       </c>
       <c r="D245">
-        <v>100315.4843839374</v>
+        <v>100315.650627429</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -3824,13 +3824,13 @@
         <v>38139.84722222222</v>
       </c>
       <c r="B246">
-        <v>292.0251474200432</v>
+        <v>291.7455023622242</v>
       </c>
       <c r="C246">
-        <v>0.01089704161550452</v>
+        <v>0.01089120134014149</v>
       </c>
       <c r="D246">
-        <v>100315.5034176362</v>
+        <v>100315.66412888</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -3838,13 +3838,13 @@
         <v>38139.85069444445</v>
       </c>
       <c r="B247">
-        <v>291.9613545685971</v>
+        <v>291.6711735729033</v>
       </c>
       <c r="C247">
-        <v>0.01091821626346138</v>
+        <v>0.01091157681852855</v>
       </c>
       <c r="D247">
-        <v>100315.5169286354</v>
+        <v>100315.6806993572</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -3852,13 +3852,13 @@
         <v>38139.85416666666</v>
       </c>
       <c r="B248">
-        <v>291.9492336267325</v>
+        <v>291.6703598155767</v>
       </c>
       <c r="C248">
-        <v>0.01094585608102792</v>
+        <v>0.01093918268307038</v>
       </c>
       <c r="D248">
-        <v>100315.4968110781</v>
+        <v>100315.6573739315</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -3866,13 +3866,13 @@
         <v>38139.85763888889</v>
       </c>
       <c r="B249">
-        <v>291.9111300695157</v>
+        <v>291.6172612909016</v>
       </c>
       <c r="C249">
-        <v>0.01094534815898576</v>
+        <v>0.01094024816986963</v>
       </c>
       <c r="D249">
-        <v>100315.4615456984</v>
+        <v>100315.6279918964</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -3880,13 +3880,13 @@
         <v>38139.86111111111</v>
       </c>
       <c r="B250">
-        <v>291.9320864766065</v>
+        <v>291.8164036040959</v>
       </c>
       <c r="C250">
-        <v>0.01096051057903951</v>
+        <v>0.01097674080304618</v>
       </c>
       <c r="D250">
-        <v>100315.3765598959</v>
+        <v>100315.5146747695</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -3894,13 +3894,13 @@
         <v>38139.86458333334</v>
       </c>
       <c r="B251">
-        <v>291.9342601249045</v>
+        <v>291.8006585528551</v>
       </c>
       <c r="C251">
-        <v>0.01099597738359309</v>
+        <v>0.01102244279510083</v>
       </c>
       <c r="D251">
-        <v>100315.2569058487</v>
+        <v>100315.4647485698</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -3908,13 +3908,13 @@
         <v>38139.86805555555</v>
       </c>
       <c r="B252">
-        <v>291.9994818956589</v>
+        <v>291.8135822282005</v>
       </c>
       <c r="C252">
-        <v>0.01105076772515246</v>
+        <v>0.01107177246017912</v>
       </c>
       <c r="D252">
-        <v>100315.0643876723</v>
+        <v>100315.3929806414</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -3922,13 +3922,13 @@
         <v>38139.87152777778</v>
       </c>
       <c r="B253">
-        <v>292.2202331449583</v>
+        <v>291.7064763089119</v>
       </c>
       <c r="C253">
-        <v>0.01111359601060632</v>
+        <v>0.01111350461682869</v>
       </c>
       <c r="D253">
-        <v>100314.8230126157</v>
+        <v>100315.3779813225</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -3936,13 +3936,13 @@
         <v>38139.875</v>
       </c>
       <c r="B254">
-        <v>292.3499360661673</v>
+        <v>291.7144150281116</v>
       </c>
       <c r="C254">
-        <v>0.01117870208597967</v>
+        <v>0.01115274784246044</v>
       </c>
       <c r="D254">
-        <v>100314.6105261559</v>
+        <v>100315.3070830587</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -3950,13 +3950,13 @@
         <v>38139.87847222222</v>
       </c>
       <c r="B255">
-        <v>292.3526684535812</v>
+        <v>291.5954449907363</v>
       </c>
       <c r="C255">
-        <v>0.01123867461248517</v>
+        <v>0.01118515557158307</v>
       </c>
       <c r="D255">
-        <v>100314.7236550342</v>
+        <v>100315.4682396284</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -3964,13 +3964,13 @@
         <v>38139.88194444445</v>
       </c>
       <c r="B256">
-        <v>292.3734216382882</v>
+        <v>291.6003016974633</v>
       </c>
       <c r="C256">
-        <v>0.01128939251994049</v>
+        <v>0.01121651205780201</v>
       </c>
       <c r="D256">
-        <v>100315.0235032682</v>
+        <v>100315.6871593919</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -3978,13 +3978,13 @@
         <v>38139.88541666666</v>
       </c>
       <c r="B257">
-        <v>292.2666749661579</v>
+        <v>291.4381434901795</v>
       </c>
       <c r="C257">
-        <v>0.01131659132633338</v>
+        <v>0.01123182492077842</v>
       </c>
       <c r="D257">
-        <v>100315.6270387384</v>
+        <v>100316.1725651399</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -3992,13 +3992,13 @@
         <v>38139.88888888889</v>
       </c>
       <c r="B258">
-        <v>292.110254240862</v>
+        <v>291.3711562208509</v>
       </c>
       <c r="C258">
-        <v>0.01130013030087633</v>
+        <v>0.01122091796021683</v>
       </c>
       <c r="D258">
-        <v>100316.2661290304</v>
+        <v>100316.7082046553</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4006,13 +4006,13 @@
         <v>38139.89236111111</v>
       </c>
       <c r="B259">
-        <v>291.855212618936</v>
+        <v>291.1174337237378</v>
       </c>
       <c r="C259">
-        <v>0.01124099720386149</v>
+        <v>0.01116931426246152</v>
       </c>
       <c r="D259">
-        <v>100316.8059753117</v>
+        <v>100317.2127362894</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4020,13 +4020,13 @@
         <v>38139.89583333334</v>
       </c>
       <c r="B260">
-        <v>291.6655091592758</v>
+        <v>291.0283819685635</v>
       </c>
       <c r="C260">
-        <v>0.01116197313272416</v>
+        <v>0.01110121503641384</v>
       </c>
       <c r="D260">
-        <v>100317.2205440265</v>
+        <v>100317.607752377</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4034,13 +4034,13 @@
         <v>38139.89930555555</v>
       </c>
       <c r="B261">
-        <v>291.4526395634079</v>
+        <v>290.7883916310303</v>
       </c>
       <c r="C261">
-        <v>0.01108258032728648</v>
+        <v>0.01102527506472618</v>
       </c>
       <c r="D261">
-        <v>100317.582290473</v>
+        <v>100317.9762671166</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4048,13 +4048,13 @@
         <v>38139.90277777778</v>
       </c>
       <c r="B262">
-        <v>291.3124986571331</v>
+        <v>290.7459187237499</v>
       </c>
       <c r="C262">
-        <v>0.01100722237422134</v>
+        <v>0.01095741501221787</v>
       </c>
       <c r="D262">
-        <v>100317.9031852741</v>
+        <v>100318.2746857891</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4062,13 +4062,13 @@
         <v>38139.90625</v>
       </c>
       <c r="B263">
-        <v>291.1157368336276</v>
+        <v>290.5201917145521</v>
       </c>
       <c r="C263">
-        <v>0.01092758719548235</v>
+        <v>0.01088176854371103</v>
       </c>
       <c r="D263">
-        <v>100318.2282897212</v>
+        <v>100318.5968479956</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4076,13 +4076,13 @@
         <v>38139.90972222222</v>
       </c>
       <c r="B264">
-        <v>290.9770994412635</v>
+        <v>290.4925208447129</v>
       </c>
       <c r="C264">
-        <v>0.01084715402600045</v>
+        <v>0.01080922899964991</v>
       </c>
       <c r="D264">
-        <v>100318.5346095048</v>
+        <v>100318.8703267519</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4090,13 +4090,13 @@
         <v>38139.91319444445</v>
       </c>
       <c r="B265">
-        <v>290.7728062179319</v>
+        <v>290.2555034136727</v>
       </c>
       <c r="C265">
-        <v>0.01077122644838019</v>
+        <v>0.01073667219248788</v>
       </c>
       <c r="D265">
-        <v>100318.8533613136</v>
+        <v>100319.1823110496</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4104,13 +4104,13 @@
         <v>38139.91666666666</v>
       </c>
       <c r="B266">
-        <v>290.6346410606214</v>
+        <v>290.2357875614126</v>
       </c>
       <c r="C266">
-        <v>0.01069123702661443</v>
+        <v>0.01066310240646526</v>
       </c>
       <c r="D266">
-        <v>100319.1533142667</v>
+        <v>100319.4427798439</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4118,13 +4118,13 @@
         <v>38139.92013888889</v>
       </c>
       <c r="B267">
-        <v>290.459724100783</v>
+        <v>290.0155413648963</v>
       </c>
       <c r="C267">
-        <v>0.01061510598204559</v>
+        <v>0.01058914402768809</v>
       </c>
       <c r="D267">
-        <v>100319.3624534195</v>
+        <v>100319.6486515159</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4132,13 +4132,13 @@
         <v>38139.92361111111</v>
       </c>
       <c r="B268">
-        <v>290.3815311783482</v>
+        <v>290.0533968326054</v>
       </c>
       <c r="C268">
-        <v>0.01054864452461445</v>
+        <v>0.01052735058900654</v>
       </c>
       <c r="D268">
-        <v>100319.5045559349</v>
+        <v>100319.7538332656</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4146,13 +4146,13 @@
         <v>38139.92708333334</v>
       </c>
       <c r="B269">
-        <v>290.2644123808194</v>
+        <v>289.8723718977212</v>
       </c>
       <c r="C269">
-        <v>0.01048366001849717</v>
+        <v>0.01046299567297326</v>
       </c>
       <c r="D269">
-        <v>100319.6360120443</v>
+        <v>100319.888856762</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4160,13 +4160,13 @@
         <v>38139.93055555555</v>
       </c>
       <c r="B270">
-        <v>290.23124544393</v>
+        <v>289.9470590485467</v>
       </c>
       <c r="C270">
-        <v>0.01042580630319945</v>
+        <v>0.01040820607493243</v>
       </c>
       <c r="D270">
-        <v>100319.7329847557</v>
+        <v>100319.9530626888</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -4174,13 +4174,13 @@
         <v>38139.93402777778</v>
       </c>
       <c r="B271">
-        <v>290.1471889285428</v>
+        <v>289.7798854028978</v>
       </c>
       <c r="C271">
-        <v>0.01038009327303265</v>
+        <v>0.01036222792901099</v>
       </c>
       <c r="D271">
-        <v>100319.8352196283</v>
+        <v>100320.0681055861</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4188,13 +4188,13 @@
         <v>38139.9375</v>
       </c>
       <c r="B272">
-        <v>290.1431462578002</v>
+        <v>289.876489006319</v>
       </c>
       <c r="C272">
-        <v>0.01033077048541809</v>
+        <v>0.01031605204564491</v>
       </c>
       <c r="D272">
-        <v>100319.9108036795</v>
+        <v>100320.1178876547</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4202,13 +4202,13 @@
         <v>38139.94097222222</v>
       </c>
       <c r="B273">
-        <v>289.705067821706</v>
+        <v>289.7077830749173</v>
       </c>
       <c r="C273">
-        <v>0.01019952805816495</v>
+        <v>0.01027141586627717</v>
       </c>
       <c r="D273">
-        <v>100320.1629851486</v>
+        <v>100320.2284975492</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4216,13 +4216,13 @@
         <v>38139.94444444445</v>
       </c>
       <c r="B274">
-        <v>289.2912654118143</v>
+        <v>289.817148665697</v>
       </c>
       <c r="C274">
-        <v>0.01005569329705866</v>
+        <v>0.01023794718275507</v>
       </c>
       <c r="D274">
-        <v>100320.4047769657</v>
+        <v>100320.2730754315</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4230,13 +4230,13 @@
         <v>38139.94791666666</v>
       </c>
       <c r="B275">
-        <v>289.2454077982752</v>
+        <v>289.6406926305937</v>
       </c>
       <c r="C275">
-        <v>0.009956346175356477</v>
+        <v>0.01019659397542805</v>
       </c>
       <c r="D275">
-        <v>100320.5127908894</v>
+        <v>100320.3851237996</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4244,13 +4244,13 @@
         <v>38139.95138888889</v>
       </c>
       <c r="B276">
-        <v>289.3186123608189</v>
+        <v>289.7595122446662</v>
       </c>
       <c r="C276">
-        <v>0.009927025783616376</v>
+        <v>0.01015994492249107</v>
       </c>
       <c r="D276">
-        <v>100320.5669301858</v>
+        <v>100320.428286826</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4258,13 +4258,13 @@
         <v>38139.95486111111</v>
       </c>
       <c r="B277">
-        <v>289.2871930499275</v>
+        <v>289.5716944251373</v>
       </c>
       <c r="C277">
-        <v>0.009917886293243468</v>
+        <v>0.0101278424862416</v>
       </c>
       <c r="D277">
-        <v>100320.6428154595</v>
+        <v>100320.544640152</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4272,13 +4272,13 @@
         <v>38139.95833333334</v>
       </c>
       <c r="B278">
-        <v>289.3206032238876</v>
+        <v>289.3758402137122</v>
       </c>
       <c r="C278">
-        <v>0.009876808618852841</v>
+        <v>0.01000528358217836</v>
       </c>
       <c r="D278">
-        <v>100320.7043653386</v>
+        <v>100320.7164827924</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4286,13 +4286,13 @@
         <v>38139.96180555555</v>
       </c>
       <c r="B279">
-        <v>289.2484496902686</v>
+        <v>288.9493764009186</v>
       </c>
       <c r="C279">
-        <v>0.009844451259034982</v>
+        <v>0.009857971694376978</v>
       </c>
       <c r="D279">
-        <v>100320.738185859</v>
+        <v>100320.8783142919</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4300,13 +4300,13 @@
         <v>38139.96527777778</v>
       </c>
       <c r="B280">
-        <v>289.2771069338131</v>
+        <v>289.0359129168823</v>
       </c>
       <c r="C280">
-        <v>0.009828251189553047</v>
+        <v>0.009812170168043009</v>
       </c>
       <c r="D280">
-        <v>100320.7349860321</v>
+        <v>100320.8568241449</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4314,13 +4314,13 @@
         <v>38139.96875</v>
       </c>
       <c r="B281">
-        <v>289.2100815098284</v>
+        <v>289.0387537739466</v>
       </c>
       <c r="C281">
-        <v>0.009818042956788165</v>
+        <v>0.009804863970260438</v>
       </c>
       <c r="D281">
-        <v>100320.7585726327</v>
+        <v>100320.8603949241</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4328,13 +4328,13 @@
         <v>38139.97222222222</v>
       </c>
       <c r="B282">
-        <v>289.243225164595</v>
+        <v>289.1317634009667</v>
       </c>
       <c r="C282">
-        <v>0.009814232020712587</v>
+        <v>0.009805715245747701</v>
       </c>
       <c r="D282">
-        <v>100320.7532555424</v>
+        <v>100320.8236206717</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4342,13 +4342,13 @@
         <v>38139.97569444445</v>
       </c>
       <c r="B283">
-        <v>289.1831723785728</v>
+        <v>289.0745097611713</v>
       </c>
       <c r="C283">
-        <v>0.009810536774667067</v>
+        <v>0.009807875255189563</v>
       </c>
       <c r="D283">
-        <v>100320.7753821916</v>
+        <v>100320.8450831551</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4356,13 +4356,13 @@
         <v>38139.97916666666</v>
       </c>
       <c r="B284">
-        <v>289.2182809339965</v>
+        <v>289.1209906580095</v>
       </c>
       <c r="C284">
-        <v>0.009809748409042479</v>
+        <v>0.009808062118013208</v>
       </c>
       <c r="D284">
-        <v>100320.7687725444</v>
+        <v>100320.8299763403</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -4370,13 +4370,13 @@
         <v>38139.98263888889</v>
       </c>
       <c r="B285">
-        <v>289.1621069221021</v>
+        <v>289.0370806572953</v>
       </c>
       <c r="C285">
-        <v>0.009807926847370082</v>
+        <v>0.00980696067890203</v>
       </c>
       <c r="D285">
-        <v>100320.789480685</v>
+        <v>100320.8653313692</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4384,13 +4384,13 @@
         <v>38139.98611111111</v>
       </c>
       <c r="B286">
-        <v>289.197119634158</v>
+        <v>289.079004674002</v>
       </c>
       <c r="C286">
-        <v>0.009807869203501109</v>
+        <v>0.009805911725338876</v>
       </c>
       <c r="D286">
-        <v>100320.7823176387</v>
+        <v>100320.8551166289</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4398,13 +4398,13 @@
         <v>38139.98958333334</v>
       </c>
       <c r="B287">
-        <v>289.1433213553606</v>
+        <v>289.2299967661593</v>
       </c>
       <c r="C287">
-        <v>0.009806929416522782</v>
+        <v>0.009828945233037231</v>
       </c>
       <c r="D287">
-        <v>100320.8022999281</v>
+        <v>100320.8094644006</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -4412,13 +4412,13 @@
         <v>38139.99305555555</v>
       </c>
       <c r="B288">
-        <v>289.1774009181221</v>
+        <v>289.4419791953001</v>
       </c>
       <c r="C288">
-        <v>0.009807145721049085</v>
+        <v>0.009862085610444967</v>
       </c>
       <c r="D288">
-        <v>100320.7951233924</v>
+        <v>100320.7790780534</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -4426,13 +4426,13 @@
         <v>38139.99652777778</v>
       </c>
       <c r="B289">
-        <v>289.1255002479674</v>
+        <v>289.3136909942384</v>
       </c>
       <c r="C289">
-        <v>0.009805967221733585</v>
+        <v>0.009890299778233452</v>
       </c>
       <c r="D289">
-        <v>100320.8145825529</v>
+        <v>100320.8317944113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>